<commit_message>
Nuevas funcionalidades parte 1
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/Requerimientos.xlsx
+++ b/DOCUMENTACION/Requerimientos.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\grupo_tdm\grupotdm_admin\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75016CD-05A7-4A4D-AFF2-4AC75F3799D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A041E7F3-1A8B-4186-B5B8-6DE2D0A4CBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-510" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUERIMIENTOS" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REQUERIMIENTOS!$B$4:$F$202</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="221">
   <si>
     <t>REQUERIMIENTOS</t>
   </si>
@@ -558,6 +562,147 @@
   </si>
   <si>
     <t>El sistema debe validar que el archivo no pese mas de 300MB de peso en almacenamiento</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para dirigirse al apartado de las VPNS</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion  para dirigirse al apartado de los servidores</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para agregar un servidor</t>
+  </si>
+  <si>
+    <t>Servidores</t>
+  </si>
+  <si>
+    <t>VPNS</t>
+  </si>
+  <si>
+    <t>El usuario desea tener un buscador de servidores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea tener una opcion para ir a crear Direcciones IP LINUX </t>
+  </si>
+  <si>
+    <t>El usuario desea crear una direccion ip linux con Ip y asignacion de servidor</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para ir a crear una nueva llave VPN</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para ir a ver una llave VPN.</t>
+  </si>
+  <si>
+    <t>El usuario desea crear una llave VPN con descripcion, asignacion de ip linux, asignacion de usuario y el archivo de la VPN.</t>
+  </si>
+  <si>
+    <t>El usuario desea eliminar una asignacion de una direccion ip linux.</t>
+  </si>
+  <si>
+    <t>El usuario desea asignar una direccion ip linux .</t>
+  </si>
+  <si>
+    <t>El usuario desea eliminar una llave VPN.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea tener una opcion para visualizar los detalles de un servidor </t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opción para eliminar un servidor</t>
+  </si>
+  <si>
+    <t>El usuario desea crear un servidor con nombre MV, OS, servicio, observaciones, RAM, Vcpumu, TOTALDD, IP, SPLA RDP-TS y SPLA EXCEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea editar el nombre MV, OS, servicio, observaciones, RAM, Vcpumu, TOTALDD, IP, SPLA RDP-TS y SPLA EXCEL de un servicor </t>
+  </si>
+  <si>
+    <t>El usuario desea asignar licencias sql al servidor</t>
+  </si>
+  <si>
+    <t>El usuario desea eliminar una asignacion de licencias</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para ir a ver las licencias sql</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para crear una nueva licencia sql</t>
+  </si>
+  <si>
+    <t>El usuario desea crear una licencia sql con nombre del sql</t>
+  </si>
+  <si>
+    <t>El usuario desea tener un buscador de licencias sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea filtrar los servidores por licencia </t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para exportar los servidores en un EXCEL</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para exportar las llaves VPN.</t>
+  </si>
+  <si>
+    <t>El usuario desea tener un buscador de llaves VPN</t>
+  </si>
+  <si>
+    <t>El sistema debe validar la duplicidad de asignacion de usuario a una nueva VPN.</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para ir a ver las llaves VPN</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para ir a ver las Direcciones IP LINUX</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para eliminar una direccion ip linux</t>
+  </si>
+  <si>
+    <t>El usuario desea tener un buscador de Direcciones IP LINUX</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para eliminar una licencia sql</t>
+  </si>
+  <si>
+    <t>LICENCIAS SQL</t>
+  </si>
+  <si>
+    <t>Direcciones IP LINUX</t>
+  </si>
+  <si>
+    <t>El sistema debe validar la duplicidad de servidores por medio de la IP</t>
+  </si>
+  <si>
+    <t>El usuario desea editar el nombre, usuario y archivo de una llave VPN.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO </t>
+  </si>
+  <si>
+    <t>El sistema notificara al usuario sobre la asignacion de una llave VPN.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea tener una opcion para ir a crear una nueva red de internet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea crear una nueva red de internet con codigo, detalle, cantidad,fecha de inicio, fecha final y valor unitario </t>
+  </si>
+  <si>
+    <t>Canales y enlaces de internet</t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para dirigirse al apartado de canales y enlaces de internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea tener una opción para eliminar una red de internet </t>
+  </si>
+  <si>
+    <t>El usuario desea tener una opcion para ir a editar una red de internet</t>
+  </si>
+  <si>
+    <t>El usuario desea editar el codigo, detalle, cantidad,fecha de inicio, fecha final y el valor unitario de una red de internet</t>
   </si>
 </sst>
 </file>
@@ -593,7 +738,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,8 +823,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -789,6 +970,28 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -801,7 +1004,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -833,9 +1036,165 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -857,9 +1216,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -902,9 +1258,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -939,6 +1292,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1255,10 +1620,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F159"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B3:M202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="K110" sqref="K110"/>
+    <sheetView tabSelected="1" topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G163" sqref="G163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1266,19 +1632,27 @@
     <col min="1" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="64.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="44.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="41.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-    </row>
-    <row r="4" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+    </row>
+    <row r="4" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1294,15 +1668,20 @@
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+    </row>
+    <row r="5" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="85" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1312,14 +1691,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="86"/>
       <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1327,14 +1706,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="87"/>
       <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1342,14 +1721,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="88" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1359,14 +1738,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="89"/>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1374,14 +1753,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1389,14 +1768,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="90"/>
       <c r="E11" s="9" t="s">
         <v>23</v>
       </c>
@@ -1404,14 +1783,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="91" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -1421,14 +1800,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="42"/>
+      <c r="D13" s="92"/>
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1436,14 +1815,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="42"/>
+      <c r="D14" s="92"/>
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1451,14 +1830,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="42"/>
+      <c r="D15" s="92"/>
       <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1466,14 +1845,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>12</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
@@ -1481,14 +1860,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>13</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="94" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1498,14 +1877,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="45"/>
+      <c r="D18" s="95"/>
       <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1513,14 +1892,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>15</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="45"/>
+      <c r="D19" s="95"/>
       <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1528,14 +1907,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>16</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="45"/>
+      <c r="D20" s="95"/>
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1543,14 +1922,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>17</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="45"/>
+      <c r="D21" s="95"/>
       <c r="E21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1558,14 +1937,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <v>18</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="45"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1573,14 +1952,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>19</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="45"/>
+      <c r="D23" s="95"/>
       <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1588,59 +1967,74 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
         <v>20</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C24" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="95"/>
+      <c r="E24" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="98"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="99"/>
+    </row>
+    <row r="25" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>21</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="95"/>
+      <c r="E25" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="99"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="99"/>
+      <c r="M25" s="99"/>
+    </row>
+    <row r="26" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
         <v>22</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="95"/>
+      <c r="E26" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="99"/>
+      <c r="J26" s="99"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="99"/>
+      <c r="M26" s="99"/>
+    </row>
+    <row r="27" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <v>23</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="45"/>
+      <c r="C27" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="95"/>
       <c r="E27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1648,14 +2042,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
         <v>24</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="45"/>
+      <c r="C28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="95"/>
       <c r="E28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1663,14 +2057,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>25</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="45"/>
+      <c r="C29" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="95"/>
       <c r="E29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1678,14 +2072,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7">
         <v>26</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="45"/>
+      <c r="C30" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="95"/>
       <c r="E30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1693,14 +2087,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
         <v>27</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="45"/>
+      <c r="C31" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="95"/>
       <c r="E31" s="1" t="s">
         <v>23</v>
       </c>
@@ -1708,14 +2102,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
         <v>28</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="45"/>
+      <c r="C32" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="95"/>
       <c r="E32" s="1" t="s">
         <v>23</v>
       </c>
@@ -1723,46 +2117,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
         <v>29</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="46"/>
-      <c r="E33" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="95"/>
+      <c r="E33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7">
         <v>30</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C34" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="95"/>
+      <c r="E34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
         <v>31</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="21"/>
+      <c r="C35" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="95"/>
       <c r="E35" s="1" t="s">
         <v>23</v>
       </c>
@@ -1770,44 +2162,46 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="7">
         <v>32</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="C36" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="96"/>
+      <c r="E36" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
         <v>33</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="7">
         <v>34</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="21"/>
+      <c r="C38" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="72"/>
       <c r="E38" s="1" t="s">
         <v>23</v>
       </c>
@@ -1815,14 +2209,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4">
         <v>35</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="21"/>
+      <c r="C39" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="72"/>
       <c r="E39" s="1" t="s">
         <v>23</v>
       </c>
@@ -1830,14 +2224,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7">
         <v>36</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="21"/>
+      <c r="C40" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="72"/>
       <c r="E40" s="1" t="s">
         <v>23</v>
       </c>
@@ -1845,14 +2239,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
         <v>37</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="21"/>
+      <c r="C41" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="72"/>
       <c r="E41" s="1" t="s">
         <v>23</v>
       </c>
@@ -1860,26 +2254,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
         <v>38</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="21"/>
+      <c r="C42" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="72"/>
+      <c r="E42" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="F42" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4">
         <v>39</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="21"/>
+      <c r="C43" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="72"/>
       <c r="E43" s="1" t="s">
         <v>23</v>
       </c>
@@ -1887,14 +2284,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="7">
         <v>40</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="21"/>
+      <c r="C44" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="72"/>
       <c r="E44" s="1" t="s">
         <v>23</v>
       </c>
@@ -1902,29 +2299,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
         <v>41</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="C45" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="72"/>
       <c r="F45" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="7">
         <v>42</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="21"/>
+      <c r="C46" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="72"/>
       <c r="E46" s="1" t="s">
         <v>23</v>
       </c>
@@ -1932,31 +2326,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
         <v>43</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="72"/>
+      <c r="E47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
         <v>44</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="23"/>
+      <c r="C48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="72"/>
       <c r="E48" s="1" t="s">
         <v>23</v>
       </c>
@@ -1964,14 +2356,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4">
         <v>45</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D49" s="23"/>
+      <c r="C49" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="72"/>
       <c r="E49" s="1" t="s">
         <v>23</v>
       </c>
@@ -1979,24 +2371,31 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="7">
         <v>46</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="23"/>
-      <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4">
         <v>47</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D51" s="23"/>
+      <c r="C51" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="74"/>
       <c r="E51" s="1" t="s">
         <v>23</v>
       </c>
@@ -2004,14 +2403,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="7">
         <v>48</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="23"/>
+      <c r="C52" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="74"/>
       <c r="E52" s="1" t="s">
         <v>23</v>
       </c>
@@ -2019,29 +2418,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
         <v>49</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="23"/>
-      <c r="E53" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="74"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="7">
         <v>50</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D54" s="23"/>
+      <c r="C54" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D54" s="74"/>
       <c r="E54" s="1" t="s">
         <v>23</v>
       </c>
@@ -2049,14 +2443,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4">
         <v>51</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="23"/>
+      <c r="C55" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D55" s="74"/>
       <c r="E55" s="1" t="s">
         <v>23</v>
       </c>
@@ -2064,14 +2458,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="7">
         <v>52</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="23"/>
+      <c r="C56" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="74"/>
       <c r="E56" s="1" t="s">
         <v>23</v>
       </c>
@@ -2079,14 +2473,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="4">
         <v>53</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="23"/>
+      <c r="C57" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="74"/>
       <c r="E57" s="1" t="s">
         <v>23</v>
       </c>
@@ -2094,14 +2488,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="7">
         <v>54</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="23"/>
+      <c r="C58" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="74"/>
       <c r="E58" s="1" t="s">
         <v>23</v>
       </c>
@@ -2109,14 +2503,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4">
         <v>55</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="23"/>
+      <c r="C59" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="74"/>
       <c r="E59" s="1" t="s">
         <v>23</v>
       </c>
@@ -2124,14 +2518,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="7">
         <v>56</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" s="23"/>
+      <c r="C60" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" s="74"/>
       <c r="E60" s="1" t="s">
         <v>23</v>
       </c>
@@ -2139,14 +2533,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="4">
         <v>57</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D61" s="23"/>
+      <c r="C61" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="74"/>
       <c r="E61" s="1" t="s">
         <v>23</v>
       </c>
@@ -2154,14 +2548,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="7">
         <v>58</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" s="23"/>
+      <c r="C62" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="74"/>
       <c r="E62" s="1" t="s">
         <v>23</v>
       </c>
@@ -2169,14 +2563,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="4">
         <v>59</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D63" s="23"/>
+      <c r="C63" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="74"/>
       <c r="E63" s="1" t="s">
         <v>23</v>
       </c>
@@ -2184,14 +2578,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="7">
         <v>60</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D64" s="23"/>
+      <c r="C64" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" s="74"/>
       <c r="E64" s="1" t="s">
         <v>23</v>
       </c>
@@ -2199,14 +2593,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" ht="57.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
         <v>61</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D65" s="23"/>
+      <c r="C65" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="74"/>
       <c r="E65" s="1" t="s">
         <v>23</v>
       </c>
@@ -2214,14 +2608,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="7">
         <v>62</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D66" s="23"/>
+      <c r="C66" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" s="74"/>
       <c r="E66" s="1" t="s">
         <v>23</v>
       </c>
@@ -2229,34 +2623,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="4">
         <v>63</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D67" s="23"/>
-      <c r="F67" s="8"/>
-    </row>
-    <row r="68" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="74"/>
+      <c r="E67" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="7">
         <v>64</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D68" s="23"/>
-      <c r="F68" s="8"/>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="74"/>
+      <c r="E68" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
         <v>65</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D69" s="23"/>
+      <c r="C69" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="74"/>
       <c r="E69" s="1" t="s">
         <v>23</v>
       </c>
@@ -2264,44 +2668,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="7">
         <v>66</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D70" s="23"/>
-      <c r="E70" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C70" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="D70" s="74"/>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
         <v>67</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="23"/>
-      <c r="E71" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D71" s="74"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="7">
         <v>68</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D72" s="23"/>
+      <c r="C72" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="74"/>
       <c r="E72" s="1" t="s">
         <v>23</v>
       </c>
@@ -2309,14 +2703,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="4">
         <v>69</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D73" s="23"/>
+      <c r="C73" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D73" s="74"/>
       <c r="E73" s="1" t="s">
         <v>23</v>
       </c>
@@ -2324,14 +2718,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="7">
         <v>70</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D74" s="23"/>
+      <c r="C74" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D74" s="74"/>
       <c r="E74" s="1" t="s">
         <v>23</v>
       </c>
@@ -2339,14 +2733,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="4">
         <v>71</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D75" s="23"/>
+      <c r="C75" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="74"/>
       <c r="E75" s="1" t="s">
         <v>23</v>
       </c>
@@ -2354,14 +2748,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="7">
         <v>72</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D76" s="23"/>
+      <c r="C76" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D76" s="74"/>
       <c r="E76" s="1" t="s">
         <v>23</v>
       </c>
@@ -2369,111 +2763,111 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="4">
         <v>73</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D77" s="23"/>
-      <c r="F77" s="8"/>
-    </row>
-    <row r="78" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="74"/>
+      <c r="E77" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="7">
         <v>74</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D78" s="23"/>
-      <c r="F78" s="8"/>
-    </row>
-    <row r="79" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="11">
+      <c r="C78" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="74"/>
+      <c r="E78" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="4">
         <v>75</v>
       </c>
-      <c r="C79" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D79" s="24"/>
-      <c r="E79" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F79" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="4">
+      <c r="C79" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D79" s="74"/>
+      <c r="E79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="7">
         <v>76</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D80" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C80" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D80" s="74"/>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="4">
         <v>77</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D81" s="26"/>
-      <c r="E81" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D81" s="74"/>
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="7">
         <v>78</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D82" s="26"/>
-      <c r="E82" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C82" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D82" s="75"/>
+      <c r="E82" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="4">
         <v>79</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D83" s="26"/>
-      <c r="E83" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="7">
         <v>80</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D84" s="26"/>
+      <c r="C84" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="77"/>
       <c r="E84" s="1" t="s">
         <v>23</v>
       </c>
@@ -2481,14 +2875,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="4">
         <v>81</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D85" s="26"/>
+      <c r="C85" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D85" s="77"/>
       <c r="E85" s="1" t="s">
         <v>23</v>
       </c>
@@ -2496,14 +2890,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="7">
         <v>82</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D86" s="26"/>
+      <c r="C86" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D86" s="77"/>
       <c r="E86" s="1" t="s">
         <v>23</v>
       </c>
@@ -2511,14 +2905,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="4">
         <v>83</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D87" s="26"/>
+      <c r="C87" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D87" s="77"/>
       <c r="E87" s="1" t="s">
         <v>23</v>
       </c>
@@ -2526,14 +2920,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="7">
         <v>84</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D88" s="26"/>
+      <c r="C88" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D88" s="77"/>
       <c r="E88" s="1" t="s">
         <v>23</v>
       </c>
@@ -2541,14 +2935,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="4">
         <v>85</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D89" s="26"/>
+      <c r="C89" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D89" s="77"/>
       <c r="E89" s="1" t="s">
         <v>23</v>
       </c>
@@ -2556,14 +2950,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="7">
         <v>86</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D90" s="26"/>
+      <c r="C90" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90" s="77"/>
       <c r="E90" s="1" t="s">
         <v>23</v>
       </c>
@@ -2571,14 +2965,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="4">
         <v>87</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D91" s="26"/>
+      <c r="C91" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D91" s="77"/>
       <c r="E91" s="1" t="s">
         <v>23</v>
       </c>
@@ -2586,14 +2980,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="7">
         <v>88</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D92" s="26"/>
+      <c r="C92" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D92" s="77"/>
       <c r="E92" s="1" t="s">
         <v>23</v>
       </c>
@@ -2601,14 +2995,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6" ht="57.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="4">
         <v>89</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D93" s="26"/>
+      <c r="C93" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" s="77"/>
       <c r="E93" s="1" t="s">
         <v>23</v>
       </c>
@@ -2616,14 +3010,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="7">
         <v>90</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D94" s="26"/>
+      <c r="C94" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D94" s="77"/>
       <c r="E94" s="1" t="s">
         <v>23</v>
       </c>
@@ -2631,14 +3025,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="4">
         <v>91</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D95" s="26"/>
+      <c r="C95" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D95" s="77"/>
       <c r="E95" s="1" t="s">
         <v>23</v>
       </c>
@@ -2646,14 +3040,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="7">
         <v>92</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D96" s="26"/>
+      <c r="C96" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D96" s="77"/>
       <c r="E96" s="1" t="s">
         <v>23</v>
       </c>
@@ -2661,46 +3055,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="11">
+    <row r="97" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="4">
         <v>93</v>
       </c>
-      <c r="C97" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D97" s="27"/>
-      <c r="E97" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F97" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="4">
+      <c r="C97" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D97" s="77"/>
+      <c r="E97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="7">
         <v>94</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D98" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F98" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C98" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D98" s="77"/>
+      <c r="E98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="4">
         <v>95</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D99" s="29"/>
+      <c r="C99" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D99" s="77"/>
       <c r="E99" s="1" t="s">
         <v>23</v>
       </c>
@@ -2708,44 +3100,46 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="7">
         <v>96</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D100" s="29"/>
-      <c r="E100" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F100" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="C100" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D100" s="78"/>
+      <c r="E100" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="4">
         <v>97</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D101" s="29"/>
-      <c r="E101" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F101" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D101" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="7">
         <v>98</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D102" s="29"/>
+      <c r="C102" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D102" s="80"/>
       <c r="E102" s="1" t="s">
         <v>23</v>
       </c>
@@ -2753,14 +3147,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="4">
         <v>99</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D103" s="29"/>
+      <c r="C103" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D103" s="80"/>
       <c r="E103" s="1" t="s">
         <v>23</v>
       </c>
@@ -2768,14 +3162,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="7">
         <v>100</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D104" s="29"/>
+      <c r="C104" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D104" s="80"/>
       <c r="E104" s="1" t="s">
         <v>23</v>
       </c>
@@ -2783,14 +3177,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4">
         <v>101</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D105" s="29"/>
+      <c r="C105" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D105" s="80"/>
       <c r="E105" s="1" t="s">
         <v>23</v>
       </c>
@@ -2798,14 +3192,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="7">
         <v>102</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D106" s="29"/>
+      <c r="C106" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D106" s="80"/>
       <c r="E106" s="1" t="s">
         <v>23</v>
       </c>
@@ -2813,14 +3207,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="4">
         <v>103</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D107" s="29"/>
+      <c r="C107" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D107" s="80"/>
       <c r="E107" s="1" t="s">
         <v>23</v>
       </c>
@@ -2828,14 +3222,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="7">
         <v>104</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D108" s="29"/>
+      <c r="C108" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D108" s="80"/>
       <c r="E108" s="1" t="s">
         <v>23</v>
       </c>
@@ -2843,14 +3237,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="4">
         <v>105</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D109" s="29"/>
+      <c r="C109" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" s="80"/>
       <c r="E109" s="1" t="s">
         <v>23</v>
       </c>
@@ -2858,14 +3252,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="7">
         <v>106</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D110" s="29"/>
+      <c r="C110" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D110" s="80"/>
       <c r="E110" s="1" t="s">
         <v>23</v>
       </c>
@@ -2873,14 +3267,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="4">
         <v>107</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D111" s="29"/>
+      <c r="C111" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D111" s="80"/>
       <c r="E111" s="1" t="s">
         <v>23</v>
       </c>
@@ -2888,14 +3282,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="7">
         <v>108</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D112" s="29"/>
+      <c r="C112" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D112" s="80"/>
       <c r="E112" s="1" t="s">
         <v>23</v>
       </c>
@@ -2903,14 +3297,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="4">
         <v>109</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D113" s="29"/>
+      <c r="C113" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D113" s="80"/>
       <c r="E113" s="1" t="s">
         <v>23</v>
       </c>
@@ -2918,14 +3312,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B114" s="7">
         <v>110</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D114" s="29"/>
+      <c r="C114" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D114" s="80"/>
       <c r="E114" s="1" t="s">
         <v>23</v>
       </c>
@@ -2933,14 +3327,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="4">
         <v>111</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D115" s="29"/>
+      <c r="C115" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D115" s="80"/>
       <c r="E115" s="1" t="s">
         <v>23</v>
       </c>
@@ -2948,14 +3342,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="7">
         <v>112</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D116" s="29"/>
+      <c r="C116" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D116" s="80"/>
       <c r="E116" s="1" t="s">
         <v>23</v>
       </c>
@@ -2963,14 +3357,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="4">
         <v>113</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D117" s="29"/>
+      <c r="C117" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D117" s="80"/>
       <c r="E117" s="1" t="s">
         <v>23</v>
       </c>
@@ -2978,14 +3372,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="7">
         <v>114</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D118" s="29"/>
+      <c r="C118" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D118" s="80"/>
       <c r="E118" s="1" t="s">
         <v>23</v>
       </c>
@@ -2993,14 +3387,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="4">
         <v>115</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D119" s="29"/>
+      <c r="C119" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D119" s="80"/>
       <c r="E119" s="1" t="s">
         <v>23</v>
       </c>
@@ -3008,46 +3402,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="7">
         <v>116</v>
       </c>
-      <c r="C120" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D120" s="30"/>
-      <c r="E120" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F120" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C120" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D120" s="80"/>
+      <c r="E120" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B121" s="4">
         <v>117</v>
       </c>
-      <c r="C121" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D121" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F121" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C121" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D121" s="80"/>
+      <c r="E121" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F121" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="7">
         <v>118</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D122" s="32"/>
+      <c r="C122" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D122" s="80"/>
       <c r="E122" s="1" t="s">
         <v>23</v>
       </c>
@@ -3055,44 +3447,46 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="4">
         <v>119</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D123" s="32"/>
-      <c r="E123" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F123" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C123" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D123" s="81"/>
+      <c r="E123" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="7">
         <v>120</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D124" s="32"/>
-      <c r="E124" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F124" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C124" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D124" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="4">
         <v>121</v>
       </c>
-      <c r="C125" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D125" s="32"/>
+      <c r="C125" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D125" s="83"/>
       <c r="E125" s="1" t="s">
         <v>23</v>
       </c>
@@ -3100,14 +3494,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="7">
         <v>122</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D126" s="32"/>
+      <c r="C126" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D126" s="83"/>
       <c r="E126" s="1" t="s">
         <v>23</v>
       </c>
@@ -3115,14 +3509,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="4">
         <v>123</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D127" s="32"/>
+      <c r="C127" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D127" s="83"/>
       <c r="E127" s="1" t="s">
         <v>23</v>
       </c>
@@ -3130,14 +3524,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="7">
         <v>124</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D128" s="32"/>
+      <c r="C128" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D128" s="83"/>
       <c r="E128" s="1" t="s">
         <v>23</v>
       </c>
@@ -3145,14 +3539,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="4">
         <v>125</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D129" s="32"/>
+      <c r="C129" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D129" s="83"/>
       <c r="E129" s="1" t="s">
         <v>23</v>
       </c>
@@ -3160,14 +3554,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="7">
         <v>126</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D130" s="32"/>
+      <c r="C130" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D130" s="83"/>
       <c r="E130" s="1" t="s">
         <v>23</v>
       </c>
@@ -3175,46 +3569,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="4">
         <v>127</v>
       </c>
-      <c r="C131" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D131" s="33"/>
-      <c r="E131" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F131" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C131" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D131" s="83"/>
+      <c r="E131" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F131" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B132" s="7">
         <v>128</v>
       </c>
-      <c r="C132" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D132" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E132" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F132" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C132" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D132" s="83"/>
+      <c r="E132" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F132" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B133" s="4">
         <v>129</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D133" s="13"/>
+      <c r="C133" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D133" s="83"/>
       <c r="E133" s="1" t="s">
         <v>23</v>
       </c>
@@ -3222,44 +3614,46 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="7">
         <v>130</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D134" s="13"/>
-      <c r="E134" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F134" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="135" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C134" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D134" s="84"/>
+      <c r="E134" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F134" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="4">
         <v>131</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D135" s="13"/>
-      <c r="E135" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F135" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="136" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D135" s="64" t="s">
+        <v>164</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="7">
         <v>132</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D136" s="13"/>
+      <c r="C136" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D136" s="65"/>
       <c r="E136" s="1" t="s">
         <v>23</v>
       </c>
@@ -3267,14 +3661,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="4">
         <v>133</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D137" s="13"/>
+      <c r="C137" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D137" s="65"/>
       <c r="E137" s="1" t="s">
         <v>23</v>
       </c>
@@ -3282,14 +3676,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="7">
         <v>134</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D138" s="13"/>
+      <c r="C138" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D138" s="65"/>
       <c r="E138" s="1" t="s">
         <v>23</v>
       </c>
@@ -3297,14 +3691,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="4">
         <v>135</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D139" s="13"/>
+      <c r="C139" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D139" s="65"/>
       <c r="E139" s="1" t="s">
         <v>23</v>
       </c>
@@ -3312,14 +3706,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="7">
         <v>136</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D140" s="13"/>
+      <c r="C140" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D140" s="65"/>
       <c r="E140" s="1" t="s">
         <v>23</v>
       </c>
@@ -3327,14 +3721,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B141" s="4">
         <v>137</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D141" s="13"/>
+      <c r="C141" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D141" s="65"/>
       <c r="E141" s="1" t="s">
         <v>23</v>
       </c>
@@ -3342,14 +3736,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="7">
         <v>138</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D142" s="13"/>
+      <c r="C142" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D142" s="65"/>
       <c r="E142" s="1" t="s">
         <v>23</v>
       </c>
@@ -3357,14 +3751,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="4">
         <v>139</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D143" s="13"/>
+      <c r="C143" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D143" s="65"/>
       <c r="E143" s="1" t="s">
         <v>23</v>
       </c>
@@ -3372,14 +3766,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="7">
         <v>140</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D144" s="13"/>
+      <c r="C144" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D144" s="65"/>
       <c r="E144" s="1" t="s">
         <v>23</v>
       </c>
@@ -3387,14 +3781,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="4">
         <v>141</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D145" s="13"/>
+      <c r="C145" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D145" s="65"/>
       <c r="E145" s="1" t="s">
         <v>23</v>
       </c>
@@ -3402,14 +3796,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="7">
         <v>142</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D146" s="13"/>
+      <c r="C146" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D146" s="65"/>
       <c r="E146" s="1" t="s">
         <v>23</v>
       </c>
@@ -3417,14 +3811,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B147" s="4">
         <v>143</v>
       </c>
-      <c r="C147" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D147" s="13"/>
+      <c r="C147" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D147" s="65"/>
       <c r="E147" s="1" t="s">
         <v>23</v>
       </c>
@@ -3432,14 +3826,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B148" s="7">
         <v>144</v>
       </c>
-      <c r="C148" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D148" s="13"/>
+      <c r="C148" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D148" s="65"/>
       <c r="E148" s="1" t="s">
         <v>23</v>
       </c>
@@ -3447,14 +3841,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="4">
         <v>145</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D149" s="13"/>
+      <c r="C149" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D149" s="65"/>
       <c r="E149" s="1" t="s">
         <v>23</v>
       </c>
@@ -3462,14 +3856,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B150" s="7">
         <v>146</v>
       </c>
-      <c r="C150" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D150" s="13"/>
+      <c r="C150" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D150" s="65"/>
       <c r="E150" s="1" t="s">
         <v>23</v>
       </c>
@@ -3477,14 +3871,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="4">
         <v>147</v>
       </c>
-      <c r="C151" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D151" s="13"/>
+      <c r="C151" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D151" s="65"/>
       <c r="E151" s="1" t="s">
         <v>23</v>
       </c>
@@ -3492,14 +3886,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B152" s="7">
         <v>148</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D152" s="13"/>
+      <c r="C152" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D152" s="65"/>
       <c r="E152" s="1" t="s">
         <v>23</v>
       </c>
@@ -3507,132 +3901,1017 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="4">
         <v>149</v>
       </c>
-      <c r="C153" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D153" s="14"/>
-      <c r="E153" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F153" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="154" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C153" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D153" s="65"/>
+      <c r="E153" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F153" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B154" s="7">
         <v>150</v>
       </c>
-      <c r="C154" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D154" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="E154" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F154" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="155" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C154" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D154" s="65"/>
+      <c r="E154" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F154" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="4">
         <v>151</v>
       </c>
-      <c r="C155" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D155" s="16"/>
-      <c r="E155" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F155" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="156" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C155" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D155" s="65"/>
+      <c r="E155" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F155" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="7">
         <v>152</v>
       </c>
-      <c r="C156" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D156" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="E156" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F156" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C156" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D156" s="66"/>
+      <c r="E156" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F156" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="4">
         <v>153</v>
       </c>
-      <c r="C157" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D157" s="18"/>
-      <c r="E157" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F157" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="158" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C157" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D157" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F157" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="158" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="7">
         <v>154</v>
       </c>
-      <c r="C158" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D158" s="18"/>
-      <c r="E158" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F158" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="159" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C158" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D158" s="68"/>
+      <c r="E158" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F158" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="4">
         <v>155</v>
       </c>
-      <c r="C159" s="9" t="s">
+      <c r="C159" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D159" s="69" t="s">
+        <v>172</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="160" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="7">
+        <v>156</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D160" s="70"/>
+      <c r="E160" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F160" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="161" spans="2:13" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B161" s="4">
+        <v>157</v>
+      </c>
+      <c r="C161" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D161" s="70"/>
+      <c r="E161" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F161" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="162" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B162" s="7">
+        <v>158</v>
+      </c>
+      <c r="C162" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D159" s="19"/>
-      <c r="E159" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F159" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="D162" s="70"/>
+      <c r="E162" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F162" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="163" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B163" s="4">
+        <v>159</v>
+      </c>
+      <c r="C163" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="D163" s="61" t="s">
+        <v>177</v>
+      </c>
+      <c r="E163" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I163" s="99"/>
+      <c r="J163" s="99"/>
+      <c r="K163" s="100"/>
+      <c r="L163" s="99"/>
+      <c r="M163" s="99"/>
+    </row>
+    <row r="164" spans="2:13" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="7">
+        <v>160</v>
+      </c>
+      <c r="C164" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="D164" s="62"/>
+      <c r="E164" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F164" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I164" s="99"/>
+      <c r="J164" s="99"/>
+      <c r="K164" s="100"/>
+      <c r="L164" s="99"/>
+      <c r="M164" s="99"/>
+    </row>
+    <row r="165" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B165" s="4">
+        <v>161</v>
+      </c>
+      <c r="C165" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="D165" s="62"/>
+      <c r="E165" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F165" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I165" s="99"/>
+      <c r="J165" s="99"/>
+      <c r="K165" s="100"/>
+      <c r="L165" s="99"/>
+      <c r="M165" s="99"/>
+    </row>
+    <row r="166" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="7">
+        <v>162</v>
+      </c>
+      <c r="C166" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="D166" s="62"/>
+      <c r="E166" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F166" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I166" s="99"/>
+      <c r="J166" s="99"/>
+      <c r="K166" s="100"/>
+      <c r="L166" s="99"/>
+      <c r="M166" s="99"/>
+    </row>
+    <row r="167" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B167" s="4">
+        <v>163</v>
+      </c>
+      <c r="C167" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="D167" s="62"/>
+      <c r="E167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F167" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I167" s="99"/>
+      <c r="J167" s="99"/>
+      <c r="K167" s="100"/>
+      <c r="L167" s="99"/>
+      <c r="M167" s="99"/>
+    </row>
+    <row r="168" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="7">
+        <v>164</v>
+      </c>
+      <c r="C168" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D168" s="62"/>
+      <c r="E168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F168" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I168" s="99"/>
+      <c r="J168" s="99"/>
+      <c r="K168" s="100"/>
+      <c r="L168" s="99"/>
+      <c r="M168" s="99"/>
+    </row>
+    <row r="169" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B169" s="4">
+        <v>165</v>
+      </c>
+      <c r="C169" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="D169" s="62"/>
+      <c r="E169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F169" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I169" s="99"/>
+      <c r="J169" s="99"/>
+      <c r="K169" s="100"/>
+      <c r="L169" s="99"/>
+      <c r="M169" s="99"/>
+    </row>
+    <row r="170" spans="2:13" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="7">
+        <v>166</v>
+      </c>
+      <c r="C170" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="D170" s="62"/>
+      <c r="E170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F170" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I170" s="99"/>
+      <c r="J170" s="99"/>
+      <c r="K170" s="100"/>
+      <c r="L170" s="99"/>
+      <c r="M170" s="99"/>
+    </row>
+    <row r="171" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B171" s="4">
+        <v>167</v>
+      </c>
+      <c r="C171" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="D171" s="62"/>
+      <c r="E171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F171" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I171" s="99"/>
+      <c r="J171" s="99"/>
+      <c r="K171" s="100"/>
+      <c r="L171" s="99"/>
+      <c r="M171" s="99"/>
+    </row>
+    <row r="172" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="7">
+        <v>168</v>
+      </c>
+      <c r="C172" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="D172" s="62"/>
+      <c r="E172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F172" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I172" s="99"/>
+      <c r="J172" s="99"/>
+      <c r="K172" s="100"/>
+      <c r="L172" s="99"/>
+      <c r="M172" s="99"/>
+    </row>
+    <row r="173" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B173" s="4">
+        <v>169</v>
+      </c>
+      <c r="C173" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="D173" s="62"/>
+      <c r="E173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F173" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I173" s="99"/>
+      <c r="J173" s="99"/>
+      <c r="K173" s="100"/>
+      <c r="L173" s="99"/>
+      <c r="M173" s="99"/>
+    </row>
+    <row r="174" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="7">
+        <v>170</v>
+      </c>
+      <c r="C174" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D174" s="62"/>
+      <c r="E174" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F174" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I174" s="99"/>
+      <c r="J174" s="99"/>
+      <c r="K174" s="100"/>
+      <c r="L174" s="99"/>
+      <c r="M174" s="99"/>
+    </row>
+    <row r="175" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="4">
+        <v>171</v>
+      </c>
+      <c r="C175" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="D175" s="60"/>
+      <c r="E175" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F175" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I175" s="99"/>
+      <c r="J175" s="99"/>
+      <c r="K175" s="100"/>
+      <c r="L175" s="99"/>
+      <c r="M175" s="99"/>
+    </row>
+    <row r="176" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B176" s="7">
+        <v>172</v>
+      </c>
+      <c r="C176" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="D176" s="61" t="s">
+        <v>209</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I176" s="99"/>
+      <c r="J176" s="99"/>
+      <c r="K176" s="100"/>
+      <c r="L176" s="99"/>
+      <c r="M176" s="99"/>
+    </row>
+    <row r="177" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B177" s="4">
+        <v>173</v>
+      </c>
+      <c r="C177" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="D177" s="62"/>
+      <c r="E177" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F177" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I177" s="99"/>
+      <c r="J177" s="99"/>
+      <c r="K177" s="100"/>
+      <c r="L177" s="99"/>
+      <c r="M177" s="99"/>
+    </row>
+    <row r="178" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B178" s="7">
+        <v>174</v>
+      </c>
+      <c r="C178" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="D178" s="62"/>
+      <c r="E178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F178" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I178" s="99"/>
+      <c r="J178" s="99"/>
+      <c r="K178" s="100"/>
+      <c r="L178" s="99"/>
+      <c r="M178" s="99"/>
+    </row>
+    <row r="179" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B179" s="4">
+        <v>175</v>
+      </c>
+      <c r="C179" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="D179" s="62"/>
+      <c r="E179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F179" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I179" s="99"/>
+      <c r="J179" s="99"/>
+      <c r="K179" s="100"/>
+      <c r="L179" s="99"/>
+      <c r="M179" s="99"/>
+    </row>
+    <row r="180" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="7">
+        <v>176</v>
+      </c>
+      <c r="C180" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="D180" s="60"/>
+      <c r="E180" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F180" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I180" s="99"/>
+      <c r="J180" s="99"/>
+      <c r="K180" s="100"/>
+      <c r="L180" s="99"/>
+      <c r="M180" s="99"/>
+    </row>
+    <row r="181" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B181" s="4">
+        <v>177</v>
+      </c>
+      <c r="C181" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="D181" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="E181" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F181" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I181" s="99"/>
+      <c r="J181" s="99"/>
+      <c r="K181" s="100"/>
+      <c r="L181" s="99"/>
+      <c r="M181" s="99"/>
+    </row>
+    <row r="182" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="7">
+        <v>178</v>
+      </c>
+      <c r="C182" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="D182" s="62"/>
+      <c r="E182" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F182" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I182" s="99"/>
+      <c r="J182" s="99"/>
+      <c r="K182" s="100"/>
+      <c r="L182" s="99"/>
+      <c r="M182" s="99"/>
+    </row>
+    <row r="183" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B183" s="4">
+        <v>179</v>
+      </c>
+      <c r="C183" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="D183" s="62"/>
+      <c r="E183" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F183" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I183" s="99"/>
+      <c r="J183" s="99"/>
+      <c r="K183" s="100"/>
+      <c r="L183" s="99"/>
+      <c r="M183" s="99"/>
+    </row>
+    <row r="184" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="7">
+        <v>180</v>
+      </c>
+      <c r="C184" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="D184" s="62"/>
+      <c r="E184" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F184" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I184" s="99"/>
+      <c r="J184" s="99"/>
+      <c r="K184" s="100"/>
+      <c r="L184" s="99"/>
+      <c r="M184" s="99"/>
+    </row>
+    <row r="185" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="4">
+        <v>181</v>
+      </c>
+      <c r="C185" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="D185" s="60"/>
+      <c r="E185" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F185" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I185" s="99"/>
+      <c r="J185" s="99"/>
+      <c r="K185" s="100"/>
+      <c r="L185" s="99"/>
+      <c r="M185" s="99"/>
+    </row>
+    <row r="186" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="7">
+        <v>182</v>
+      </c>
+      <c r="C186" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="D186" s="61" t="s">
+        <v>178</v>
+      </c>
+      <c r="E186" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F186" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I186" s="99"/>
+      <c r="J186" s="99"/>
+      <c r="K186" s="100"/>
+      <c r="L186" s="99"/>
+      <c r="M186" s="99"/>
+    </row>
+    <row r="187" spans="2:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="4">
+        <v>183</v>
+      </c>
+      <c r="C187" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D187" s="62"/>
+      <c r="E187" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F187" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I187" s="99"/>
+      <c r="J187" s="99"/>
+      <c r="K187" s="100"/>
+      <c r="L187" s="99"/>
+      <c r="M187" s="99"/>
+    </row>
+    <row r="188" spans="2:13" ht="156.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B188" s="7">
+        <v>184</v>
+      </c>
+      <c r="C188" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="D188" s="62"/>
+      <c r="E188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F188" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I188" s="99"/>
+      <c r="J188" s="99"/>
+      <c r="K188" s="100"/>
+      <c r="L188" s="99"/>
+      <c r="M188" s="99"/>
+    </row>
+    <row r="189" spans="2:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="4">
+        <v>185</v>
+      </c>
+      <c r="C189" s="53" t="s">
+        <v>202</v>
+      </c>
+      <c r="D189" s="62"/>
+      <c r="E189" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F189" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I189" s="99"/>
+      <c r="J189" s="99"/>
+      <c r="K189" s="100"/>
+      <c r="L189" s="99"/>
+      <c r="M189" s="99"/>
+    </row>
+    <row r="190" spans="2:13" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="7">
+        <v>186</v>
+      </c>
+      <c r="C190" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="D190" s="62"/>
+      <c r="E190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F190" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I190" s="99"/>
+      <c r="J190" s="99"/>
+      <c r="K190" s="100"/>
+      <c r="L190" s="99"/>
+      <c r="M190" s="99"/>
+    </row>
+    <row r="191" spans="2:13" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="4">
+        <v>187</v>
+      </c>
+      <c r="C191" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="D191" s="62"/>
+      <c r="E191" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F191" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I191" s="99"/>
+      <c r="J191" s="99"/>
+      <c r="K191" s="100"/>
+      <c r="L191" s="99"/>
+      <c r="M191" s="99"/>
+    </row>
+    <row r="192" spans="2:13" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="7">
+        <v>188</v>
+      </c>
+      <c r="C192" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="D192" s="62"/>
+      <c r="E192" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F192" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I192" s="99"/>
+      <c r="J192" s="99"/>
+      <c r="K192" s="100"/>
+      <c r="L192" s="99"/>
+      <c r="M192" s="99"/>
+    </row>
+    <row r="193" spans="2:13" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B193" s="4">
+        <v>189</v>
+      </c>
+      <c r="C193" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="D193" s="62"/>
+      <c r="E193" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F193" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I193" s="99"/>
+      <c r="J193" s="99"/>
+      <c r="K193" s="100"/>
+      <c r="L193" s="99"/>
+      <c r="M193" s="99"/>
+    </row>
+    <row r="194" spans="2:13" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="7">
+        <v>190</v>
+      </c>
+      <c r="C194" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="D194" s="62"/>
+      <c r="E194" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F194" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I194" s="99"/>
+      <c r="J194" s="99"/>
+      <c r="K194" s="100"/>
+      <c r="L194" s="99"/>
+      <c r="M194" s="99"/>
+    </row>
+    <row r="195" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B195" s="4">
+        <v>191</v>
+      </c>
+      <c r="C195" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="D195" s="62"/>
+      <c r="E195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F195" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I195" s="99"/>
+      <c r="J195" s="99"/>
+      <c r="K195" s="100"/>
+      <c r="L195" s="99"/>
+      <c r="M195" s="99"/>
+    </row>
+    <row r="196" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="7">
+        <v>192</v>
+      </c>
+      <c r="C196" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="D196" s="62"/>
+      <c r="E196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F196" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I196" s="99"/>
+      <c r="J196" s="99"/>
+      <c r="K196" s="100"/>
+      <c r="L196" s="99"/>
+      <c r="M196" s="99"/>
+    </row>
+    <row r="197" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="4">
+        <v>193</v>
+      </c>
+      <c r="C197" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="D197" s="62"/>
+      <c r="E197" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F197" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I197" s="99"/>
+      <c r="J197" s="99"/>
+      <c r="K197" s="100"/>
+      <c r="L197" s="99"/>
+      <c r="M197" s="99"/>
+    </row>
+    <row r="198" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="4">
+        <v>194</v>
+      </c>
+      <c r="C198" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="D198" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="E198" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F198" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="I198" s="99"/>
+      <c r="J198" s="99"/>
+      <c r="K198" s="100"/>
+      <c r="L198" s="99"/>
+      <c r="M198" s="99"/>
+    </row>
+    <row r="199" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="4">
+        <v>195</v>
+      </c>
+      <c r="C199" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="D199" s="60"/>
+      <c r="E199" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F199" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I199" s="99"/>
+      <c r="J199" s="99"/>
+      <c r="K199" s="100"/>
+      <c r="L199" s="99"/>
+      <c r="M199" s="99"/>
+    </row>
+    <row r="200" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="7">
+        <v>196</v>
+      </c>
+      <c r="C200" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="D200" s="60"/>
+      <c r="E200" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F200" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I200" s="99"/>
+      <c r="J200" s="99"/>
+      <c r="K200" s="100"/>
+      <c r="L200" s="99"/>
+      <c r="M200" s="99"/>
+    </row>
+    <row r="201" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B201" s="4">
+        <v>197</v>
+      </c>
+      <c r="C201" s="57" t="s">
+        <v>219</v>
+      </c>
+      <c r="D201" s="60"/>
+      <c r="E201" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F201" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I201" s="99"/>
+      <c r="J201" s="99"/>
+      <c r="K201" s="100"/>
+      <c r="L201" s="99"/>
+      <c r="M201" s="99"/>
+    </row>
+    <row r="202" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B202" s="45">
+        <v>198</v>
+      </c>
+      <c r="C202" s="58" t="s">
+        <v>220</v>
+      </c>
+      <c r="D202" s="60"/>
+      <c r="E202" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F202" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I202" s="99"/>
+      <c r="J202" s="99"/>
+      <c r="K202" s="100"/>
+      <c r="L202" s="99"/>
+      <c r="M202" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <autoFilter ref="B4:F202" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <mergeCells count="24">
+    <mergeCell ref="D83:D100"/>
+    <mergeCell ref="D101:D123"/>
+    <mergeCell ref="D124:D134"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="D17:D33"/>
-    <mergeCell ref="D132:D153"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="D156:D159"/>
-    <mergeCell ref="D34:D46"/>
-    <mergeCell ref="D47:D79"/>
-    <mergeCell ref="D80:D97"/>
-    <mergeCell ref="D98:D120"/>
-    <mergeCell ref="D121:D131"/>
+    <mergeCell ref="D17:D36"/>
+    <mergeCell ref="D198:D202"/>
+    <mergeCell ref="K186:K197"/>
+    <mergeCell ref="K198:K202"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="K163:K175"/>
+    <mergeCell ref="K176:K180"/>
+    <mergeCell ref="K181:K185"/>
+    <mergeCell ref="D163:D175"/>
+    <mergeCell ref="D176:D180"/>
+    <mergeCell ref="D181:D185"/>
+    <mergeCell ref="D186:D197"/>
+    <mergeCell ref="D135:D156"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="D159:D162"/>
+    <mergeCell ref="D37:D49"/>
+    <mergeCell ref="D50:D82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBCF908-77BD-4BA6-9374-C5B0B97F8B99}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Nuevas funcionalidades parte 2
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/Requerimientos.xlsx
+++ b/DOCUMENTACION/Requerimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\grupo_tdm\grupotdm_admin\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A041E7F3-1A8B-4186-B5B8-6DE2D0A4CBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C5C33-34BC-4B05-8B25-962371870DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-510" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,9 +615,6 @@
     <t>El usuario desea crear un servidor con nombre MV, OS, servicio, observaciones, RAM, Vcpumu, TOTALDD, IP, SPLA RDP-TS y SPLA EXCEL</t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario desea editar el nombre MV, OS, servicio, observaciones, RAM, Vcpumu, TOTALDD, IP, SPLA RDP-TS y SPLA EXCEL de un servicor </t>
-  </si>
-  <si>
     <t>El usuario desea asignar licencias sql al servidor</t>
   </si>
   <si>
@@ -636,9 +633,6 @@
     <t>El usuario desea tener un buscador de licencias sql</t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario desea filtrar los servidores por licencia </t>
-  </si>
-  <si>
     <t>El usuario desea tener una opcion para exportar los servidores en un EXCEL</t>
   </si>
   <si>
@@ -703,13 +697,19 @@
   </si>
   <si>
     <t>El usuario desea editar el codigo, detalle, cantidad,fecha de inicio, fecha final y el valor unitario de una red de internet</t>
+  </si>
+  <si>
+    <t>El usuario desea filtrar los estados del servidor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario desea editar el nombre MV, OS, servicio, observaciones, RAM, Vcpumu, TOTALDD,, SPLA RDP-TS y SPLA EXCEL de un servicor </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,6 +732,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bahnschrift SemiBold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Bahnschrift SemiBold"/>
@@ -1180,21 +1187,93 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1231,79 +1310,7 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1623,8 +1630,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B3:M202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G163" sqref="G163"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1639,18 +1646,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
     </row>
     <row r="4" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1668,11 +1675,11 @@
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
     </row>
     <row r="5" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -1681,7 +1688,7 @@
       <c r="C5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="70" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1698,7 +1705,7 @@
       <c r="C6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="86"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1713,7 +1720,7 @@
       <c r="C7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="87"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1728,7 +1735,7 @@
       <c r="C8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="88" t="s">
+      <c r="D8" s="73" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1745,7 +1752,7 @@
       <c r="C9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="89"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1760,7 +1767,7 @@
       <c r="C10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="89"/>
+      <c r="D10" s="74"/>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1775,7 +1782,7 @@
       <c r="C11" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="90"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="9" t="s">
         <v>23</v>
       </c>
@@ -1790,7 +1797,7 @@
       <c r="C12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="91" t="s">
+      <c r="D12" s="76" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -1807,7 +1814,7 @@
       <c r="C13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="92"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1822,7 +1829,7 @@
       <c r="C14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="92"/>
+      <c r="D14" s="77"/>
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1837,7 +1844,7 @@
       <c r="C15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="92"/>
+      <c r="D15" s="77"/>
       <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1852,7 +1859,7 @@
       <c r="C16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="93"/>
+      <c r="D16" s="78"/>
       <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
@@ -1867,7 +1874,7 @@
       <c r="C17" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="94" t="s">
+      <c r="D17" s="79" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1884,7 +1891,7 @@
       <c r="C18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="95"/>
+      <c r="D18" s="80"/>
       <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1899,7 +1906,7 @@
       <c r="C19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="95"/>
+      <c r="D19" s="80"/>
       <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1914,7 +1921,7 @@
       <c r="C20" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="95"/>
+      <c r="D20" s="80"/>
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1929,7 +1936,7 @@
       <c r="C21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="95"/>
+      <c r="D21" s="80"/>
       <c r="E21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1944,7 +1951,7 @@
       <c r="C22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="95"/>
+      <c r="D22" s="80"/>
       <c r="E22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1966,7 @@
       <c r="C23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="95"/>
+      <c r="D23" s="80"/>
       <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1967,74 +1974,74 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>20</v>
       </c>
       <c r="C24" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="D24" s="95"/>
+      <c r="D24" s="80"/>
       <c r="E24" s="27" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="99"/>
-      <c r="J24" s="99"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="99"/>
-      <c r="M24" s="99"/>
-    </row>
-    <row r="25" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+    </row>
+    <row r="25" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>21</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="D25" s="95"/>
+        <v>215</v>
+      </c>
+      <c r="D25" s="80"/>
       <c r="E25" s="27" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="99"/>
-      <c r="J25" s="99"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="99"/>
-      <c r="M25" s="99"/>
-    </row>
-    <row r="26" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+    </row>
+    <row r="26" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <v>22</v>
       </c>
       <c r="C26" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="95"/>
+      <c r="D26" s="80"/>
       <c r="E26" s="27" t="s">
         <v>23</v>
       </c>
       <c r="F26" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="99"/>
-      <c r="J26" s="99"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="99"/>
-      <c r="M26" s="99"/>
-    </row>
-    <row r="27" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+    </row>
+    <row r="27" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>23</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="95"/>
+      <c r="D27" s="80"/>
       <c r="E27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2042,14 +2049,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
         <v>24</v>
       </c>
       <c r="C28" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="95"/>
+      <c r="D28" s="80"/>
       <c r="E28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2057,14 +2064,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>25</v>
       </c>
       <c r="C29" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="95"/>
+      <c r="D29" s="80"/>
       <c r="E29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2072,14 +2079,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
         <v>26</v>
       </c>
       <c r="C30" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="95"/>
+      <c r="D30" s="80"/>
       <c r="E30" s="1" t="s">
         <v>23</v>
       </c>
@@ -2087,14 +2094,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>27</v>
       </c>
       <c r="C31" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="95"/>
+      <c r="D31" s="80"/>
       <c r="E31" s="1" t="s">
         <v>23</v>
       </c>
@@ -2102,14 +2109,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7">
         <v>28</v>
       </c>
       <c r="C32" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="95"/>
+      <c r="D32" s="80"/>
       <c r="E32" s="1" t="s">
         <v>23</v>
       </c>
@@ -2117,14 +2124,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>29</v>
       </c>
       <c r="C33" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="95"/>
+      <c r="D33" s="80"/>
       <c r="E33" s="1" t="s">
         <v>23</v>
       </c>
@@ -2132,14 +2139,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7">
         <v>30</v>
       </c>
       <c r="C34" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="95"/>
+      <c r="D34" s="80"/>
       <c r="E34" s="1" t="s">
         <v>23</v>
       </c>
@@ -2147,14 +2154,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>31</v>
       </c>
       <c r="C35" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="95"/>
+      <c r="D35" s="80"/>
       <c r="E35" s="1" t="s">
         <v>23</v>
       </c>
@@ -2169,7 +2176,7 @@
       <c r="C36" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="96"/>
+      <c r="D36" s="81"/>
       <c r="E36" s="9" t="s">
         <v>23</v>
       </c>
@@ -2177,14 +2184,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>33</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="71" t="s">
+      <c r="D37" s="95" t="s">
         <v>54</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -2194,14 +2201,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7">
         <v>34</v>
       </c>
       <c r="C38" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="72"/>
+      <c r="D38" s="96"/>
       <c r="E38" s="1" t="s">
         <v>23</v>
       </c>
@@ -2209,14 +2216,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>35</v>
       </c>
       <c r="C39" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="72"/>
+      <c r="D39" s="96"/>
       <c r="E39" s="1" t="s">
         <v>23</v>
       </c>
@@ -2224,14 +2231,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7">
         <v>36</v>
       </c>
       <c r="C40" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="72"/>
+      <c r="D40" s="96"/>
       <c r="E40" s="1" t="s">
         <v>23</v>
       </c>
@@ -2239,14 +2246,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
         <v>37</v>
       </c>
       <c r="C41" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="72"/>
+      <c r="D41" s="96"/>
       <c r="E41" s="1" t="s">
         <v>23</v>
       </c>
@@ -2254,14 +2261,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="7">
         <v>38</v>
       </c>
       <c r="C42" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="72"/>
+      <c r="D42" s="96"/>
       <c r="E42" s="1" t="s">
         <v>23</v>
       </c>
@@ -2269,14 +2276,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>39</v>
       </c>
       <c r="C43" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="72"/>
+      <c r="D43" s="96"/>
       <c r="E43" s="1" t="s">
         <v>23</v>
       </c>
@@ -2284,14 +2291,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7">
         <v>40</v>
       </c>
       <c r="C44" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="72"/>
+      <c r="D44" s="96"/>
       <c r="E44" s="1" t="s">
         <v>23</v>
       </c>
@@ -2299,26 +2306,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>41</v>
       </c>
       <c r="C45" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="72"/>
+      <c r="D45" s="96"/>
       <c r="F45" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="7">
         <v>42</v>
       </c>
       <c r="C46" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="72"/>
+      <c r="D46" s="96"/>
       <c r="E46" s="1" t="s">
         <v>23</v>
       </c>
@@ -2326,14 +2333,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>43</v>
       </c>
       <c r="C47" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="72"/>
+      <c r="D47" s="96"/>
       <c r="E47" s="1" t="s">
         <v>23</v>
       </c>
@@ -2341,14 +2348,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7">
         <v>44</v>
       </c>
       <c r="C48" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="72"/>
+      <c r="D48" s="96"/>
       <c r="E48" s="1" t="s">
         <v>23</v>
       </c>
@@ -2356,14 +2363,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>45</v>
       </c>
       <c r="C49" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="72"/>
+      <c r="D49" s="96"/>
       <c r="E49" s="1" t="s">
         <v>23</v>
       </c>
@@ -2371,14 +2378,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
         <v>46</v>
       </c>
       <c r="C50" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="73" t="s">
+      <c r="D50" s="97" t="s">
         <v>83</v>
       </c>
       <c r="E50" s="5" t="s">
@@ -2388,14 +2395,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4">
         <v>47</v>
       </c>
       <c r="C51" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="74"/>
+      <c r="D51" s="98"/>
       <c r="E51" s="1" t="s">
         <v>23</v>
       </c>
@@ -2403,14 +2410,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
         <v>48</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D52" s="74"/>
+      <c r="D52" s="98"/>
       <c r="E52" s="1" t="s">
         <v>23</v>
       </c>
@@ -2418,24 +2425,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="4">
         <v>49</v>
       </c>
       <c r="C53" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D53" s="74"/>
+      <c r="D53" s="98"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="7">
         <v>50</v>
       </c>
       <c r="C54" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="74"/>
+      <c r="D54" s="98"/>
       <c r="E54" s="1" t="s">
         <v>23</v>
       </c>
@@ -2443,14 +2450,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="4">
         <v>51</v>
       </c>
       <c r="C55" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="74"/>
+      <c r="D55" s="98"/>
       <c r="E55" s="1" t="s">
         <v>23</v>
       </c>
@@ -2458,14 +2465,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="7">
         <v>52</v>
       </c>
       <c r="C56" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="74"/>
+      <c r="D56" s="98"/>
       <c r="E56" s="1" t="s">
         <v>23</v>
       </c>
@@ -2473,14 +2480,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4">
         <v>53</v>
       </c>
       <c r="C57" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="74"/>
+      <c r="D57" s="98"/>
       <c r="E57" s="1" t="s">
         <v>23</v>
       </c>
@@ -2488,14 +2495,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="7">
         <v>54</v>
       </c>
       <c r="C58" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="74"/>
+      <c r="D58" s="98"/>
       <c r="E58" s="1" t="s">
         <v>23</v>
       </c>
@@ -2503,14 +2510,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="4">
         <v>55</v>
       </c>
       <c r="C59" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="74"/>
+      <c r="D59" s="98"/>
       <c r="E59" s="1" t="s">
         <v>23</v>
       </c>
@@ -2518,14 +2525,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="7">
         <v>56</v>
       </c>
       <c r="C60" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D60" s="74"/>
+      <c r="D60" s="98"/>
       <c r="E60" s="1" t="s">
         <v>23</v>
       </c>
@@ -2533,14 +2540,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4">
         <v>57</v>
       </c>
       <c r="C61" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="74"/>
+      <c r="D61" s="98"/>
       <c r="E61" s="1" t="s">
         <v>23</v>
       </c>
@@ -2548,14 +2555,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="7">
         <v>58</v>
       </c>
       <c r="C62" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="74"/>
+      <c r="D62" s="98"/>
       <c r="E62" s="1" t="s">
         <v>23</v>
       </c>
@@ -2563,14 +2570,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4">
         <v>59</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="74"/>
+      <c r="D63" s="98"/>
       <c r="E63" s="1" t="s">
         <v>23</v>
       </c>
@@ -2578,14 +2585,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="7">
         <v>60</v>
       </c>
       <c r="C64" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D64" s="74"/>
+      <c r="D64" s="98"/>
       <c r="E64" s="1" t="s">
         <v>23</v>
       </c>
@@ -2593,14 +2600,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="57.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4">
         <v>61</v>
       </c>
       <c r="C65" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="74"/>
+      <c r="D65" s="98"/>
       <c r="E65" s="1" t="s">
         <v>23</v>
       </c>
@@ -2608,14 +2615,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="7">
         <v>62</v>
       </c>
       <c r="C66" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="74"/>
+      <c r="D66" s="98"/>
       <c r="E66" s="1" t="s">
         <v>23</v>
       </c>
@@ -2623,14 +2630,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="4">
         <v>63</v>
       </c>
       <c r="C67" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D67" s="74"/>
+      <c r="D67" s="98"/>
       <c r="E67" s="1" t="s">
         <v>23</v>
       </c>
@@ -2638,14 +2645,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="7">
         <v>64</v>
       </c>
       <c r="C68" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="74"/>
+      <c r="D68" s="98"/>
       <c r="E68" s="1" t="s">
         <v>23</v>
       </c>
@@ -2653,14 +2660,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4">
         <v>65</v>
       </c>
       <c r="C69" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D69" s="74"/>
+      <c r="D69" s="98"/>
       <c r="E69" s="1" t="s">
         <v>23</v>
       </c>
@@ -2668,34 +2675,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="7">
         <v>66</v>
       </c>
       <c r="C70" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="D70" s="74"/>
+      <c r="D70" s="98"/>
       <c r="F70" s="8"/>
     </row>
-    <row r="71" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4">
         <v>67</v>
       </c>
       <c r="C71" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="D71" s="74"/>
+      <c r="D71" s="98"/>
       <c r="F71" s="8"/>
     </row>
-    <row r="72" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="7">
         <v>68</v>
       </c>
       <c r="C72" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="74"/>
+      <c r="D72" s="98"/>
       <c r="E72" s="1" t="s">
         <v>23</v>
       </c>
@@ -2703,14 +2710,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4">
         <v>69</v>
       </c>
       <c r="C73" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D73" s="74"/>
+      <c r="D73" s="98"/>
       <c r="E73" s="1" t="s">
         <v>23</v>
       </c>
@@ -2718,14 +2725,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="7">
         <v>70</v>
       </c>
       <c r="C74" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="74"/>
+      <c r="D74" s="98"/>
       <c r="E74" s="1" t="s">
         <v>23</v>
       </c>
@@ -2733,14 +2740,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4">
         <v>71</v>
       </c>
       <c r="C75" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D75" s="74"/>
+      <c r="D75" s="98"/>
       <c r="E75" s="1" t="s">
         <v>23</v>
       </c>
@@ -2748,14 +2755,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="7">
         <v>72</v>
       </c>
       <c r="C76" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="74"/>
+      <c r="D76" s="98"/>
       <c r="E76" s="1" t="s">
         <v>23</v>
       </c>
@@ -2763,14 +2770,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4">
         <v>73</v>
       </c>
       <c r="C77" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D77" s="74"/>
+      <c r="D77" s="98"/>
       <c r="E77" s="1" t="s">
         <v>23</v>
       </c>
@@ -2778,14 +2785,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="7">
         <v>74</v>
       </c>
       <c r="C78" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D78" s="74"/>
+      <c r="D78" s="98"/>
       <c r="E78" s="1" t="s">
         <v>23</v>
       </c>
@@ -2793,14 +2800,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="4">
         <v>75</v>
       </c>
       <c r="C79" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D79" s="74"/>
+      <c r="D79" s="98"/>
       <c r="E79" s="1" t="s">
         <v>23</v>
       </c>
@@ -2808,24 +2815,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="7">
         <v>76</v>
       </c>
       <c r="C80" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D80" s="74"/>
+      <c r="D80" s="98"/>
       <c r="F80" s="8"/>
     </row>
-    <row r="81" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="4">
         <v>77</v>
       </c>
       <c r="C81" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D81" s="74"/>
+      <c r="D81" s="98"/>
       <c r="F81" s="8"/>
     </row>
     <row r="82" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2835,7 +2842,7 @@
       <c r="C82" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="75"/>
+      <c r="D82" s="99"/>
       <c r="E82" s="9" t="s">
         <v>23</v>
       </c>
@@ -2843,14 +2850,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4">
         <v>79</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D83" s="76" t="s">
+      <c r="D83" s="60" t="s">
         <v>103</v>
       </c>
       <c r="E83" s="5" t="s">
@@ -2860,14 +2867,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="7">
         <v>80</v>
       </c>
       <c r="C84" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D84" s="77"/>
+      <c r="D84" s="61"/>
       <c r="E84" s="1" t="s">
         <v>23</v>
       </c>
@@ -2875,14 +2882,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="4">
         <v>81</v>
       </c>
       <c r="C85" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D85" s="77"/>
+      <c r="D85" s="61"/>
       <c r="E85" s="1" t="s">
         <v>23</v>
       </c>
@@ -2890,14 +2897,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="7">
         <v>82</v>
       </c>
       <c r="C86" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D86" s="77"/>
+      <c r="D86" s="61"/>
       <c r="E86" s="1" t="s">
         <v>23</v>
       </c>
@@ -2905,14 +2912,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="4">
         <v>83</v>
       </c>
       <c r="C87" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D87" s="77"/>
+      <c r="D87" s="61"/>
       <c r="E87" s="1" t="s">
         <v>23</v>
       </c>
@@ -2920,14 +2927,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="7">
         <v>84</v>
       </c>
       <c r="C88" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D88" s="77"/>
+      <c r="D88" s="61"/>
       <c r="E88" s="1" t="s">
         <v>23</v>
       </c>
@@ -2935,14 +2942,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="4">
         <v>85</v>
       </c>
       <c r="C89" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D89" s="77"/>
+      <c r="D89" s="61"/>
       <c r="E89" s="1" t="s">
         <v>23</v>
       </c>
@@ -2950,14 +2957,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="7">
         <v>86</v>
       </c>
       <c r="C90" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D90" s="77"/>
+      <c r="D90" s="61"/>
       <c r="E90" s="1" t="s">
         <v>23</v>
       </c>
@@ -2965,14 +2972,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="4">
         <v>87</v>
       </c>
       <c r="C91" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D91" s="77"/>
+      <c r="D91" s="61"/>
       <c r="E91" s="1" t="s">
         <v>23</v>
       </c>
@@ -2980,14 +2987,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="7">
         <v>88</v>
       </c>
       <c r="C92" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D92" s="77"/>
+      <c r="D92" s="61"/>
       <c r="E92" s="1" t="s">
         <v>23</v>
       </c>
@@ -2995,14 +3002,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="57.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="4">
         <v>89</v>
       </c>
       <c r="C93" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D93" s="77"/>
+      <c r="D93" s="61"/>
       <c r="E93" s="1" t="s">
         <v>23</v>
       </c>
@@ -3010,14 +3017,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="7">
         <v>90</v>
       </c>
       <c r="C94" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D94" s="77"/>
+      <c r="D94" s="61"/>
       <c r="E94" s="1" t="s">
         <v>23</v>
       </c>
@@ -3025,14 +3032,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="4">
         <v>91</v>
       </c>
       <c r="C95" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D95" s="77"/>
+      <c r="D95" s="61"/>
       <c r="E95" s="1" t="s">
         <v>23</v>
       </c>
@@ -3040,14 +3047,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="7">
         <v>92</v>
       </c>
       <c r="C96" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D96" s="77"/>
+      <c r="D96" s="61"/>
       <c r="E96" s="1" t="s">
         <v>23</v>
       </c>
@@ -3055,14 +3062,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="4">
         <v>93</v>
       </c>
       <c r="C97" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D97" s="77"/>
+      <c r="D97" s="61"/>
       <c r="E97" s="1" t="s">
         <v>23</v>
       </c>
@@ -3070,14 +3077,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="7">
         <v>94</v>
       </c>
       <c r="C98" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D98" s="77"/>
+      <c r="D98" s="61"/>
       <c r="E98" s="1" t="s">
         <v>23</v>
       </c>
@@ -3085,14 +3092,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="4">
         <v>95</v>
       </c>
       <c r="C99" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D99" s="77"/>
+      <c r="D99" s="61"/>
       <c r="E99" s="1" t="s">
         <v>23</v>
       </c>
@@ -3107,7 +3114,7 @@
       <c r="C100" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D100" s="78"/>
+      <c r="D100" s="62"/>
       <c r="E100" s="9" t="s">
         <v>23</v>
       </c>
@@ -3115,14 +3122,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="4">
         <v>97</v>
       </c>
       <c r="C101" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D101" s="79" t="s">
+      <c r="D101" s="63" t="s">
         <v>126</v>
       </c>
       <c r="E101" s="5" t="s">
@@ -3132,14 +3139,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="7">
         <v>98</v>
       </c>
       <c r="C102" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D102" s="80"/>
+      <c r="D102" s="64"/>
       <c r="E102" s="1" t="s">
         <v>23</v>
       </c>
@@ -3147,14 +3154,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="4">
         <v>99</v>
       </c>
       <c r="C103" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D103" s="80"/>
+      <c r="D103" s="64"/>
       <c r="E103" s="1" t="s">
         <v>23</v>
       </c>
@@ -3162,14 +3169,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B104" s="7">
         <v>100</v>
       </c>
       <c r="C104" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D104" s="80"/>
+      <c r="D104" s="64"/>
       <c r="E104" s="1" t="s">
         <v>23</v>
       </c>
@@ -3177,14 +3184,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B105" s="4">
         <v>101</v>
       </c>
       <c r="C105" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D105" s="80"/>
+      <c r="D105" s="64"/>
       <c r="E105" s="1" t="s">
         <v>23</v>
       </c>
@@ -3192,14 +3199,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B106" s="7">
         <v>102</v>
       </c>
       <c r="C106" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D106" s="80"/>
+      <c r="D106" s="64"/>
       <c r="E106" s="1" t="s">
         <v>23</v>
       </c>
@@ -3207,14 +3214,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B107" s="4">
         <v>103</v>
       </c>
       <c r="C107" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D107" s="80"/>
+      <c r="D107" s="64"/>
       <c r="E107" s="1" t="s">
         <v>23</v>
       </c>
@@ -3222,14 +3229,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B108" s="7">
         <v>104</v>
       </c>
       <c r="C108" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D108" s="80"/>
+      <c r="D108" s="64"/>
       <c r="E108" s="1" t="s">
         <v>23</v>
       </c>
@@ -3237,14 +3244,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B109" s="4">
         <v>105</v>
       </c>
       <c r="C109" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D109" s="80"/>
+      <c r="D109" s="64"/>
       <c r="E109" s="1" t="s">
         <v>23</v>
       </c>
@@ -3252,14 +3259,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B110" s="7">
         <v>106</v>
       </c>
       <c r="C110" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D110" s="80"/>
+      <c r="D110" s="64"/>
       <c r="E110" s="1" t="s">
         <v>23</v>
       </c>
@@ -3267,14 +3274,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" s="4">
         <v>107</v>
       </c>
       <c r="C111" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D111" s="80"/>
+      <c r="D111" s="64"/>
       <c r="E111" s="1" t="s">
         <v>23</v>
       </c>
@@ -3282,14 +3289,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B112" s="7">
         <v>108</v>
       </c>
       <c r="C112" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="D112" s="80"/>
+      <c r="D112" s="64"/>
       <c r="E112" s="1" t="s">
         <v>23</v>
       </c>
@@ -3297,14 +3304,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B113" s="4">
         <v>109</v>
       </c>
       <c r="C113" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D113" s="80"/>
+      <c r="D113" s="64"/>
       <c r="E113" s="1" t="s">
         <v>23</v>
       </c>
@@ -3312,14 +3319,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B114" s="7">
         <v>110</v>
       </c>
       <c r="C114" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D114" s="80"/>
+      <c r="D114" s="64"/>
       <c r="E114" s="1" t="s">
         <v>23</v>
       </c>
@@ -3327,14 +3334,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B115" s="4">
         <v>111</v>
       </c>
       <c r="C115" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="D115" s="80"/>
+      <c r="D115" s="64"/>
       <c r="E115" s="1" t="s">
         <v>23</v>
       </c>
@@ -3342,14 +3349,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B116" s="7">
         <v>112</v>
       </c>
       <c r="C116" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D116" s="80"/>
+      <c r="D116" s="64"/>
       <c r="E116" s="1" t="s">
         <v>23</v>
       </c>
@@ -3357,14 +3364,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B117" s="4">
         <v>113</v>
       </c>
       <c r="C117" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D117" s="80"/>
+      <c r="D117" s="64"/>
       <c r="E117" s="1" t="s">
         <v>23</v>
       </c>
@@ -3372,14 +3379,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B118" s="7">
         <v>114</v>
       </c>
       <c r="C118" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D118" s="80"/>
+      <c r="D118" s="64"/>
       <c r="E118" s="1" t="s">
         <v>23</v>
       </c>
@@ -3387,14 +3394,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" s="4">
         <v>115</v>
       </c>
       <c r="C119" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D119" s="80"/>
+      <c r="D119" s="64"/>
       <c r="E119" s="1" t="s">
         <v>23</v>
       </c>
@@ -3402,14 +3409,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B120" s="7">
         <v>116</v>
       </c>
       <c r="C120" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D120" s="80"/>
+      <c r="D120" s="64"/>
       <c r="E120" s="1" t="s">
         <v>23</v>
       </c>
@@ -3417,14 +3424,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121" s="4">
         <v>117</v>
       </c>
       <c r="C121" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D121" s="80"/>
+      <c r="D121" s="64"/>
       <c r="E121" s="1" t="s">
         <v>23</v>
       </c>
@@ -3432,14 +3439,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B122" s="7">
         <v>118</v>
       </c>
       <c r="C122" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D122" s="80"/>
+      <c r="D122" s="64"/>
       <c r="E122" s="1" t="s">
         <v>23</v>
       </c>
@@ -3454,7 +3461,7 @@
       <c r="C123" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D123" s="81"/>
+      <c r="D123" s="65"/>
       <c r="E123" s="9" t="s">
         <v>23</v>
       </c>
@@ -3462,14 +3469,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124" s="7">
         <v>120</v>
       </c>
       <c r="C124" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D124" s="82" t="s">
+      <c r="D124" s="66" t="s">
         <v>140</v>
       </c>
       <c r="E124" s="5" t="s">
@@ -3479,14 +3486,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125" s="4">
         <v>121</v>
       </c>
       <c r="C125" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="D125" s="83"/>
+      <c r="D125" s="67"/>
       <c r="E125" s="1" t="s">
         <v>23</v>
       </c>
@@ -3494,14 +3501,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B126" s="7">
         <v>122</v>
       </c>
       <c r="C126" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="D126" s="83"/>
+      <c r="D126" s="67"/>
       <c r="E126" s="1" t="s">
         <v>23</v>
       </c>
@@ -3509,14 +3516,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127" s="4">
         <v>123</v>
       </c>
       <c r="C127" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D127" s="83"/>
+      <c r="D127" s="67"/>
       <c r="E127" s="1" t="s">
         <v>23</v>
       </c>
@@ -3524,14 +3531,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128" s="7">
         <v>124</v>
       </c>
       <c r="C128" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D128" s="83"/>
+      <c r="D128" s="67"/>
       <c r="E128" s="1" t="s">
         <v>23</v>
       </c>
@@ -3539,14 +3546,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B129" s="4">
         <v>125</v>
       </c>
       <c r="C129" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D129" s="83"/>
+      <c r="D129" s="67"/>
       <c r="E129" s="1" t="s">
         <v>23</v>
       </c>
@@ -3554,14 +3561,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B130" s="7">
         <v>126</v>
       </c>
       <c r="C130" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="D130" s="83"/>
+      <c r="D130" s="67"/>
       <c r="E130" s="1" t="s">
         <v>23</v>
       </c>
@@ -3569,14 +3576,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B131" s="4">
         <v>127</v>
       </c>
       <c r="C131" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D131" s="83"/>
+      <c r="D131" s="67"/>
       <c r="E131" s="1" t="s">
         <v>23</v>
       </c>
@@ -3584,14 +3591,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B132" s="7">
         <v>128</v>
       </c>
       <c r="C132" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D132" s="83"/>
+      <c r="D132" s="67"/>
       <c r="E132" s="1" t="s">
         <v>23</v>
       </c>
@@ -3599,14 +3606,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B133" s="4">
         <v>129</v>
       </c>
       <c r="C133" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="D133" s="83"/>
+      <c r="D133" s="67"/>
       <c r="E133" s="1" t="s">
         <v>23</v>
       </c>
@@ -3621,7 +3628,7 @@
       <c r="C134" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D134" s="84"/>
+      <c r="D134" s="68"/>
       <c r="E134" s="9" t="s">
         <v>23</v>
       </c>
@@ -3629,14 +3636,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B135" s="4">
         <v>131</v>
       </c>
       <c r="C135" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D135" s="64" t="s">
+      <c r="D135" s="88" t="s">
         <v>164</v>
       </c>
       <c r="E135" s="5" t="s">
@@ -3646,14 +3653,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B136" s="7">
         <v>132</v>
       </c>
       <c r="C136" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D136" s="65"/>
+      <c r="D136" s="89"/>
       <c r="E136" s="1" t="s">
         <v>23</v>
       </c>
@@ -3661,14 +3668,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B137" s="4">
         <v>133</v>
       </c>
       <c r="C137" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D137" s="65"/>
+      <c r="D137" s="89"/>
       <c r="E137" s="1" t="s">
         <v>23</v>
       </c>
@@ -3676,14 +3683,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B138" s="7">
         <v>134</v>
       </c>
       <c r="C138" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D138" s="65"/>
+      <c r="D138" s="89"/>
       <c r="E138" s="1" t="s">
         <v>23</v>
       </c>
@@ -3691,14 +3698,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B139" s="4">
         <v>135</v>
       </c>
       <c r="C139" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="D139" s="65"/>
+      <c r="D139" s="89"/>
       <c r="E139" s="1" t="s">
         <v>23</v>
       </c>
@@ -3706,14 +3713,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B140" s="7">
         <v>136</v>
       </c>
       <c r="C140" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D140" s="65"/>
+      <c r="D140" s="89"/>
       <c r="E140" s="1" t="s">
         <v>23</v>
       </c>
@@ -3721,14 +3728,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B141" s="4">
         <v>137</v>
       </c>
       <c r="C141" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D141" s="65"/>
+      <c r="D141" s="89"/>
       <c r="E141" s="1" t="s">
         <v>23</v>
       </c>
@@ -3736,14 +3743,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="2:6" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:6" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B142" s="7">
         <v>138</v>
       </c>
       <c r="C142" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D142" s="65"/>
+      <c r="D142" s="89"/>
       <c r="E142" s="1" t="s">
         <v>23</v>
       </c>
@@ -3751,14 +3758,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B143" s="4">
         <v>139</v>
       </c>
       <c r="C143" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D143" s="65"/>
+      <c r="D143" s="89"/>
       <c r="E143" s="1" t="s">
         <v>23</v>
       </c>
@@ -3766,14 +3773,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B144" s="7">
         <v>140</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D144" s="65"/>
+      <c r="D144" s="89"/>
       <c r="E144" s="1" t="s">
         <v>23</v>
       </c>
@@ -3781,14 +3788,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B145" s="4">
         <v>141</v>
       </c>
       <c r="C145" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="D145" s="65"/>
+      <c r="D145" s="89"/>
       <c r="E145" s="1" t="s">
         <v>23</v>
       </c>
@@ -3796,14 +3803,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B146" s="7">
         <v>142</v>
       </c>
       <c r="C146" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D146" s="65"/>
+      <c r="D146" s="89"/>
       <c r="E146" s="1" t="s">
         <v>23</v>
       </c>
@@ -3811,14 +3818,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B147" s="4">
         <v>143</v>
       </c>
       <c r="C147" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D147" s="65"/>
+      <c r="D147" s="89"/>
       <c r="E147" s="1" t="s">
         <v>23</v>
       </c>
@@ -3826,14 +3833,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B148" s="7">
         <v>144</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="D148" s="65"/>
+      <c r="D148" s="89"/>
       <c r="E148" s="1" t="s">
         <v>23</v>
       </c>
@@ -3841,14 +3848,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B149" s="4">
         <v>145</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D149" s="65"/>
+      <c r="D149" s="89"/>
       <c r="E149" s="1" t="s">
         <v>23</v>
       </c>
@@ -3856,14 +3863,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B150" s="7">
         <v>146</v>
       </c>
       <c r="C150" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D150" s="65"/>
+      <c r="D150" s="89"/>
       <c r="E150" s="1" t="s">
         <v>23</v>
       </c>
@@ -3871,14 +3878,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B151" s="4">
         <v>147</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D151" s="65"/>
+      <c r="D151" s="89"/>
       <c r="E151" s="1" t="s">
         <v>23</v>
       </c>
@@ -3886,14 +3893,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B152" s="7">
         <v>148</v>
       </c>
       <c r="C152" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D152" s="65"/>
+      <c r="D152" s="89"/>
       <c r="E152" s="1" t="s">
         <v>23</v>
       </c>
@@ -3901,14 +3908,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B153" s="4">
         <v>149</v>
       </c>
       <c r="C153" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D153" s="65"/>
+      <c r="D153" s="89"/>
       <c r="E153" s="1" t="s">
         <v>23</v>
       </c>
@@ -3916,14 +3923,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B154" s="7">
         <v>150</v>
       </c>
       <c r="C154" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D154" s="65"/>
+      <c r="D154" s="89"/>
       <c r="E154" s="1" t="s">
         <v>23</v>
       </c>
@@ -3931,14 +3938,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B155" s="4">
         <v>151</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D155" s="65"/>
+      <c r="D155" s="89"/>
       <c r="E155" s="1" t="s">
         <v>23</v>
       </c>
@@ -3953,7 +3960,7 @@
       <c r="C156" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D156" s="66"/>
+      <c r="D156" s="90"/>
       <c r="E156" s="9" t="s">
         <v>23</v>
       </c>
@@ -3961,14 +3968,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B157" s="4">
         <v>153</v>
       </c>
       <c r="C157" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D157" s="67" t="s">
+      <c r="D157" s="91" t="s">
         <v>167</v>
       </c>
       <c r="E157" s="5" t="s">
@@ -3985,7 +3992,7 @@
       <c r="C158" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D158" s="68"/>
+      <c r="D158" s="92"/>
       <c r="E158" s="9" t="s">
         <v>23</v>
       </c>
@@ -3993,14 +4000,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B159" s="4">
         <v>155</v>
       </c>
       <c r="C159" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="D159" s="69" t="s">
+      <c r="D159" s="93" t="s">
         <v>172</v>
       </c>
       <c r="E159" s="5" t="s">
@@ -4010,14 +4017,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="2:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B160" s="7">
         <v>156</v>
       </c>
       <c r="C160" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="D160" s="70"/>
+      <c r="D160" s="94"/>
       <c r="E160" s="1" t="s">
         <v>23</v>
       </c>
@@ -4025,14 +4032,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="2:13" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:13" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B161" s="4">
         <v>157</v>
       </c>
       <c r="C161" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D161" s="70"/>
+      <c r="D161" s="94"/>
       <c r="E161" s="1" t="s">
         <v>23</v>
       </c>
@@ -4040,14 +4047,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B162" s="7">
         <v>158</v>
       </c>
       <c r="C162" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D162" s="70"/>
+      <c r="D162" s="94"/>
       <c r="E162" s="1" t="s">
         <v>23</v>
       </c>
@@ -4055,67 +4062,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B163" s="4">
         <v>159</v>
       </c>
       <c r="C163" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="D163" s="61" t="s">
+      <c r="D163" s="86" t="s">
         <v>177</v>
       </c>
       <c r="E163" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F163" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I163" s="99"/>
-      <c r="J163" s="99"/>
-      <c r="K163" s="100"/>
-      <c r="L163" s="99"/>
-      <c r="M163" s="99"/>
-    </row>
-    <row r="164" spans="2:13" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I163" s="27"/>
+      <c r="J163" s="27"/>
+      <c r="K163" s="84"/>
+      <c r="L163" s="27"/>
+      <c r="M163" s="27"/>
+    </row>
+    <row r="164" spans="2:13" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B164" s="7">
         <v>160</v>
       </c>
       <c r="C164" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="D164" s="62"/>
+      <c r="D164" s="87"/>
       <c r="E164" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I164" s="99"/>
-      <c r="J164" s="99"/>
-      <c r="K164" s="100"/>
-      <c r="L164" s="99"/>
-      <c r="M164" s="99"/>
-    </row>
-    <row r="165" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="I164" s="27"/>
+      <c r="J164" s="27"/>
+      <c r="K164" s="84"/>
+      <c r="L164" s="27"/>
+      <c r="M164" s="27"/>
+    </row>
+    <row r="165" spans="2:13" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B165" s="4">
         <v>161</v>
       </c>
       <c r="C165" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="D165" s="62"/>
+        <v>208</v>
+      </c>
+      <c r="D165" s="87"/>
       <c r="E165" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I165" s="99"/>
-      <c r="J165" s="99"/>
-      <c r="K165" s="100"/>
-      <c r="L165" s="99"/>
-      <c r="M165" s="99"/>
+        <v>23</v>
+      </c>
+      <c r="I165" s="27"/>
+      <c r="J165" s="27"/>
+      <c r="K165" s="84"/>
+      <c r="L165" s="27"/>
+      <c r="M165" s="27"/>
     </row>
     <row r="166" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B166" s="7">
@@ -4124,198 +4131,198 @@
       <c r="C166" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="D166" s="62"/>
+      <c r="D166" s="87"/>
       <c r="E166" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F166" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I166" s="99"/>
-      <c r="J166" s="99"/>
-      <c r="K166" s="100"/>
-      <c r="L166" s="99"/>
-      <c r="M166" s="99"/>
+      <c r="I166" s="27"/>
+      <c r="J166" s="27"/>
+      <c r="K166" s="84"/>
+      <c r="L166" s="27"/>
+      <c r="M166" s="27"/>
     </row>
     <row r="167" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B167" s="4">
         <v>163</v>
       </c>
       <c r="C167" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="D167" s="62"/>
+        <v>219</v>
+      </c>
+      <c r="D167" s="87"/>
       <c r="E167" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F167" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I167" s="99"/>
-      <c r="J167" s="99"/>
-      <c r="K167" s="100"/>
-      <c r="L167" s="99"/>
-      <c r="M167" s="99"/>
+      <c r="I167" s="27"/>
+      <c r="J167" s="27"/>
+      <c r="K167" s="84"/>
+      <c r="L167" s="27"/>
+      <c r="M167" s="27"/>
     </row>
     <row r="168" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B168" s="7">
         <v>164</v>
       </c>
       <c r="C168" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="D168" s="62"/>
+        <v>197</v>
+      </c>
+      <c r="D168" s="87"/>
       <c r="E168" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F168" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I168" s="99"/>
-      <c r="J168" s="99"/>
-      <c r="K168" s="100"/>
-      <c r="L168" s="99"/>
-      <c r="M168" s="99"/>
-    </row>
-    <row r="169" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="I168" s="27"/>
+      <c r="J168" s="27"/>
+      <c r="K168" s="84"/>
+      <c r="L168" s="27"/>
+      <c r="M168" s="27"/>
+    </row>
+    <row r="169" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B169" s="4">
         <v>165</v>
       </c>
-      <c r="C169" s="44" t="s">
+      <c r="C169" s="100" t="s">
         <v>188</v>
       </c>
-      <c r="D169" s="62"/>
+      <c r="D169" s="87"/>
       <c r="E169" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I169" s="99"/>
-      <c r="J169" s="99"/>
-      <c r="K169" s="100"/>
-      <c r="L169" s="99"/>
-      <c r="M169" s="99"/>
-    </row>
-    <row r="170" spans="2:13" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I169" s="27"/>
+      <c r="J169" s="27"/>
+      <c r="K169" s="84"/>
+      <c r="L169" s="27"/>
+      <c r="M169" s="27"/>
+    </row>
+    <row r="170" spans="2:13" ht="43.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B170" s="7">
         <v>166</v>
       </c>
       <c r="C170" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="D170" s="62"/>
+        <v>220</v>
+      </c>
+      <c r="D170" s="87"/>
       <c r="E170" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I170" s="99"/>
-      <c r="J170" s="99"/>
-      <c r="K170" s="100"/>
-      <c r="L170" s="99"/>
-      <c r="M170" s="99"/>
-    </row>
-    <row r="171" spans="2:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="I170" s="27"/>
+      <c r="J170" s="27"/>
+      <c r="K170" s="84"/>
+      <c r="L170" s="27"/>
+      <c r="M170" s="27"/>
+    </row>
+    <row r="171" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B171" s="4">
         <v>167</v>
       </c>
       <c r="C171" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="D171" s="62"/>
+        <v>191</v>
+      </c>
+      <c r="D171" s="87"/>
       <c r="E171" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I171" s="99"/>
-      <c r="J171" s="99"/>
-      <c r="K171" s="100"/>
-      <c r="L171" s="99"/>
-      <c r="M171" s="99"/>
-    </row>
-    <row r="172" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I171" s="27"/>
+      <c r="J171" s="27"/>
+      <c r="K171" s="84"/>
+      <c r="L171" s="27"/>
+      <c r="M171" s="27"/>
+    </row>
+    <row r="172" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B172" s="7">
         <v>168</v>
       </c>
       <c r="C172" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="D172" s="62"/>
+        <v>192</v>
+      </c>
+      <c r="D172" s="87"/>
       <c r="E172" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I172" s="99"/>
-      <c r="J172" s="99"/>
-      <c r="K172" s="100"/>
-      <c r="L172" s="99"/>
-      <c r="M172" s="99"/>
-    </row>
-    <row r="173" spans="2:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="I172" s="27"/>
+      <c r="J172" s="27"/>
+      <c r="K172" s="84"/>
+      <c r="L172" s="27"/>
+      <c r="M172" s="27"/>
+    </row>
+    <row r="173" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B173" s="4">
         <v>169</v>
       </c>
       <c r="C173" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="D173" s="62"/>
+      <c r="D173" s="87"/>
       <c r="E173" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I173" s="99"/>
-      <c r="J173" s="99"/>
-      <c r="K173" s="100"/>
-      <c r="L173" s="99"/>
-      <c r="M173" s="99"/>
-    </row>
-    <row r="174" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I173" s="27"/>
+      <c r="J173" s="27"/>
+      <c r="K173" s="84"/>
+      <c r="L173" s="27"/>
+      <c r="M173" s="27"/>
+    </row>
+    <row r="174" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B174" s="7">
         <v>170</v>
       </c>
       <c r="C174" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="D174" s="62"/>
+        <v>193</v>
+      </c>
+      <c r="D174" s="87"/>
       <c r="E174" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I174" s="99"/>
-      <c r="J174" s="99"/>
-      <c r="K174" s="100"/>
-      <c r="L174" s="99"/>
-      <c r="M174" s="99"/>
-    </row>
-    <row r="175" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I174" s="27"/>
+      <c r="J174" s="27"/>
+      <c r="K174" s="84"/>
+      <c r="L174" s="27"/>
+      <c r="M174" s="27"/>
+    </row>
+    <row r="175" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B175" s="4">
         <v>171</v>
       </c>
       <c r="C175" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="D175" s="60"/>
+        <v>202</v>
+      </c>
+      <c r="D175" s="83"/>
       <c r="E175" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F175" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I175" s="99"/>
-      <c r="J175" s="99"/>
-      <c r="K175" s="100"/>
-      <c r="L175" s="99"/>
-      <c r="M175" s="99"/>
+        <v>23</v>
+      </c>
+      <c r="I175" s="27"/>
+      <c r="J175" s="27"/>
+      <c r="K175" s="84"/>
+      <c r="L175" s="27"/>
+      <c r="M175" s="27"/>
     </row>
     <row r="176" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="7">
@@ -4324,8 +4331,8 @@
       <c r="C176" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="D176" s="61" t="s">
-        <v>209</v>
+      <c r="D176" s="86" t="s">
+        <v>207</v>
       </c>
       <c r="E176" s="5" t="s">
         <v>23</v>
@@ -4333,31 +4340,31 @@
       <c r="F176" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I176" s="99"/>
-      <c r="J176" s="99"/>
-      <c r="K176" s="100"/>
-      <c r="L176" s="99"/>
-      <c r="M176" s="99"/>
+      <c r="I176" s="27"/>
+      <c r="J176" s="27"/>
+      <c r="K176" s="84"/>
+      <c r="L176" s="27"/>
+      <c r="M176" s="27"/>
     </row>
     <row r="177" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B177" s="4">
         <v>173</v>
       </c>
       <c r="C177" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="D177" s="62"/>
+        <v>204</v>
+      </c>
+      <c r="D177" s="87"/>
       <c r="E177" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F177" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I177" s="99"/>
-      <c r="J177" s="99"/>
-      <c r="K177" s="100"/>
-      <c r="L177" s="99"/>
-      <c r="M177" s="99"/>
+      <c r="I177" s="27"/>
+      <c r="J177" s="27"/>
+      <c r="K177" s="84"/>
+      <c r="L177" s="27"/>
+      <c r="M177" s="27"/>
     </row>
     <row r="178" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B178" s="7">
@@ -4366,18 +4373,18 @@
       <c r="C178" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="D178" s="62"/>
+      <c r="D178" s="87"/>
       <c r="E178" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F178" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I178" s="99"/>
-      <c r="J178" s="99"/>
-      <c r="K178" s="100"/>
-      <c r="L178" s="99"/>
-      <c r="M178" s="99"/>
+      <c r="I178" s="27"/>
+      <c r="J178" s="27"/>
+      <c r="K178" s="84"/>
+      <c r="L178" s="27"/>
+      <c r="M178" s="27"/>
     </row>
     <row r="179" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B179" s="4">
@@ -4386,149 +4393,149 @@
       <c r="C179" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="D179" s="62"/>
+      <c r="D179" s="87"/>
       <c r="E179" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F179" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I179" s="99"/>
-      <c r="J179" s="99"/>
-      <c r="K179" s="100"/>
-      <c r="L179" s="99"/>
-      <c r="M179" s="99"/>
+      <c r="I179" s="27"/>
+      <c r="J179" s="27"/>
+      <c r="K179" s="84"/>
+      <c r="L179" s="27"/>
+      <c r="M179" s="27"/>
     </row>
     <row r="180" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B180" s="7">
         <v>176</v>
       </c>
       <c r="C180" s="48" t="s">
-        <v>205</v>
-      </c>
-      <c r="D180" s="60"/>
+        <v>203</v>
+      </c>
+      <c r="D180" s="83"/>
       <c r="E180" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F180" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I180" s="99"/>
-      <c r="J180" s="99"/>
-      <c r="K180" s="100"/>
-      <c r="L180" s="99"/>
-      <c r="M180" s="99"/>
-    </row>
-    <row r="181" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I180" s="27"/>
+      <c r="J180" s="27"/>
+      <c r="K180" s="84"/>
+      <c r="L180" s="27"/>
+      <c r="M180" s="27"/>
+    </row>
+    <row r="181" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B181" s="4">
         <v>177</v>
       </c>
       <c r="C181" s="49" t="s">
-        <v>194</v>
-      </c>
-      <c r="D181" s="61" t="s">
-        <v>208</v>
+        <v>193</v>
+      </c>
+      <c r="D181" s="86" t="s">
+        <v>206</v>
       </c>
       <c r="E181" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F181" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I181" s="99"/>
-      <c r="J181" s="99"/>
-      <c r="K181" s="100"/>
-      <c r="L181" s="99"/>
-      <c r="M181" s="99"/>
+        <v>23</v>
+      </c>
+      <c r="I181" s="27"/>
+      <c r="J181" s="27"/>
+      <c r="K181" s="84"/>
+      <c r="L181" s="27"/>
+      <c r="M181" s="27"/>
     </row>
     <row r="182" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B182" s="7">
         <v>178</v>
       </c>
       <c r="C182" s="50" t="s">
-        <v>197</v>
-      </c>
-      <c r="D182" s="62"/>
+        <v>196</v>
+      </c>
+      <c r="D182" s="87"/>
       <c r="E182" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F182" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I182" s="99"/>
-      <c r="J182" s="99"/>
-      <c r="K182" s="100"/>
-      <c r="L182" s="99"/>
-      <c r="M182" s="99"/>
-    </row>
-    <row r="183" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="I182" s="27"/>
+      <c r="J182" s="27"/>
+      <c r="K182" s="84"/>
+      <c r="L182" s="27"/>
+      <c r="M182" s="27"/>
+    </row>
+    <row r="183" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B183" s="4">
         <v>179</v>
       </c>
       <c r="C183" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="D183" s="62"/>
+        <v>194</v>
+      </c>
+      <c r="D183" s="87"/>
       <c r="E183" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I183" s="99"/>
-      <c r="J183" s="99"/>
-      <c r="K183" s="100"/>
-      <c r="L183" s="99"/>
-      <c r="M183" s="99"/>
-    </row>
-    <row r="184" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I183" s="27"/>
+      <c r="J183" s="27"/>
+      <c r="K183" s="84"/>
+      <c r="L183" s="27"/>
+      <c r="M183" s="27"/>
+    </row>
+    <row r="184" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B184" s="7">
         <v>180</v>
       </c>
       <c r="C184" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="D184" s="62"/>
+        <v>195</v>
+      </c>
+      <c r="D184" s="87"/>
       <c r="E184" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I184" s="99"/>
-      <c r="J184" s="99"/>
-      <c r="K184" s="100"/>
-      <c r="L184" s="99"/>
-      <c r="M184" s="99"/>
-    </row>
-    <row r="185" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I184" s="27"/>
+      <c r="J184" s="27"/>
+      <c r="K184" s="84"/>
+      <c r="L184" s="27"/>
+      <c r="M184" s="27"/>
+    </row>
+    <row r="185" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B185" s="4">
         <v>181</v>
       </c>
       <c r="C185" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="D185" s="60"/>
+        <v>205</v>
+      </c>
+      <c r="D185" s="83"/>
       <c r="E185" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F185" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I185" s="99"/>
-      <c r="J185" s="99"/>
-      <c r="K185" s="100"/>
-      <c r="L185" s="99"/>
-      <c r="M185" s="99"/>
+        <v>23</v>
+      </c>
+      <c r="I185" s="27"/>
+      <c r="J185" s="27"/>
+      <c r="K185" s="84"/>
+      <c r="L185" s="27"/>
+      <c r="M185" s="27"/>
     </row>
     <row r="186" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B186" s="7">
         <v>182</v>
       </c>
       <c r="C186" s="52" t="s">
-        <v>203</v>
-      </c>
-      <c r="D186" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="D186" s="86" t="s">
         <v>178</v>
       </c>
       <c r="E186" s="5" t="s">
@@ -4537,11 +4544,11 @@
       <c r="F186" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I186" s="99"/>
-      <c r="J186" s="99"/>
-      <c r="K186" s="100"/>
-      <c r="L186" s="99"/>
-      <c r="M186" s="99"/>
+      <c r="I186" s="27"/>
+      <c r="J186" s="27"/>
+      <c r="K186" s="84"/>
+      <c r="L186" s="27"/>
+      <c r="M186" s="27"/>
     </row>
     <row r="187" spans="2:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="4">
@@ -4550,18 +4557,18 @@
       <c r="C187" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="D187" s="62"/>
+      <c r="D187" s="87"/>
       <c r="E187" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F187" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I187" s="99"/>
-      <c r="J187" s="99"/>
-      <c r="K187" s="100"/>
-      <c r="L187" s="99"/>
-      <c r="M187" s="99"/>
+      <c r="I187" s="27"/>
+      <c r="J187" s="27"/>
+      <c r="K187" s="84"/>
+      <c r="L187" s="27"/>
+      <c r="M187" s="27"/>
     </row>
     <row r="188" spans="2:13" ht="156.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B188" s="7">
@@ -4570,38 +4577,38 @@
       <c r="C188" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="D188" s="62"/>
+      <c r="D188" s="87"/>
       <c r="E188" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F188" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I188" s="99"/>
-      <c r="J188" s="99"/>
-      <c r="K188" s="100"/>
-      <c r="L188" s="99"/>
-      <c r="M188" s="99"/>
+      <c r="I188" s="27"/>
+      <c r="J188" s="27"/>
+      <c r="K188" s="84"/>
+      <c r="L188" s="27"/>
+      <c r="M188" s="27"/>
     </row>
     <row r="189" spans="2:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="4">
         <v>185</v>
       </c>
       <c r="C189" s="53" t="s">
-        <v>202</v>
-      </c>
-      <c r="D189" s="62"/>
+        <v>200</v>
+      </c>
+      <c r="D189" s="87"/>
       <c r="E189" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F189" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I189" s="99"/>
-      <c r="J189" s="99"/>
-      <c r="K189" s="100"/>
-      <c r="L189" s="99"/>
-      <c r="M189" s="99"/>
+      <c r="I189" s="27"/>
+      <c r="J189" s="27"/>
+      <c r="K189" s="84"/>
+      <c r="L189" s="27"/>
+      <c r="M189" s="27"/>
     </row>
     <row r="190" spans="2:13" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B190" s="7">
@@ -4610,78 +4617,78 @@
       <c r="C190" s="53" t="s">
         <v>183</v>
       </c>
-      <c r="D190" s="62"/>
+      <c r="D190" s="87"/>
       <c r="E190" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F190" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I190" s="99"/>
-      <c r="J190" s="99"/>
-      <c r="K190" s="100"/>
-      <c r="L190" s="99"/>
-      <c r="M190" s="99"/>
+      <c r="I190" s="27"/>
+      <c r="J190" s="27"/>
+      <c r="K190" s="84"/>
+      <c r="L190" s="27"/>
+      <c r="M190" s="27"/>
     </row>
     <row r="191" spans="2:13" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="4">
         <v>187</v>
       </c>
       <c r="C191" s="53" t="s">
-        <v>200</v>
-      </c>
-      <c r="D191" s="62"/>
+        <v>198</v>
+      </c>
+      <c r="D191" s="87"/>
       <c r="E191" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F191" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I191" s="99"/>
-      <c r="J191" s="99"/>
-      <c r="K191" s="100"/>
-      <c r="L191" s="99"/>
-      <c r="M191" s="99"/>
+      <c r="I191" s="27"/>
+      <c r="J191" s="27"/>
+      <c r="K191" s="84"/>
+      <c r="L191" s="27"/>
+      <c r="M191" s="27"/>
     </row>
     <row r="192" spans="2:13" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B192" s="7">
         <v>188</v>
       </c>
       <c r="C192" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="D192" s="62"/>
+        <v>209</v>
+      </c>
+      <c r="D192" s="87"/>
       <c r="E192" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F192" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I192" s="99"/>
-      <c r="J192" s="99"/>
-      <c r="K192" s="100"/>
-      <c r="L192" s="99"/>
-      <c r="M192" s="99"/>
+      <c r="I192" s="27"/>
+      <c r="J192" s="27"/>
+      <c r="K192" s="84"/>
+      <c r="L192" s="27"/>
+      <c r="M192" s="27"/>
     </row>
     <row r="193" spans="2:13" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="4">
         <v>189</v>
       </c>
       <c r="C193" s="53" t="s">
-        <v>201</v>
-      </c>
-      <c r="D193" s="62"/>
+        <v>199</v>
+      </c>
+      <c r="D193" s="87"/>
       <c r="E193" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F193" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I193" s="99"/>
-      <c r="J193" s="99"/>
-      <c r="K193" s="100"/>
-      <c r="L193" s="99"/>
-      <c r="M193" s="99"/>
+      <c r="I193" s="27"/>
+      <c r="J193" s="27"/>
+      <c r="K193" s="84"/>
+      <c r="L193" s="27"/>
+      <c r="M193" s="27"/>
     </row>
     <row r="194" spans="2:13" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B194" s="7">
@@ -4690,18 +4697,18 @@
       <c r="C194" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="D194" s="62"/>
+      <c r="D194" s="87"/>
       <c r="E194" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F194" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I194" s="99"/>
-      <c r="J194" s="99"/>
-      <c r="K194" s="100"/>
-      <c r="L194" s="99"/>
-      <c r="M194" s="99"/>
+      <c r="I194" s="27"/>
+      <c r="J194" s="27"/>
+      <c r="K194" s="84"/>
+      <c r="L194" s="27"/>
+      <c r="M194" s="27"/>
     </row>
     <row r="195" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B195" s="4">
@@ -4710,38 +4717,38 @@
       <c r="C195" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="D195" s="62"/>
+      <c r="D195" s="87"/>
       <c r="E195" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F195" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I195" s="99"/>
-      <c r="J195" s="99"/>
-      <c r="K195" s="100"/>
-      <c r="L195" s="99"/>
-      <c r="M195" s="99"/>
+      <c r="I195" s="27"/>
+      <c r="J195" s="27"/>
+      <c r="K195" s="84"/>
+      <c r="L195" s="27"/>
+      <c r="M195" s="27"/>
     </row>
     <row r="196" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B196" s="7">
         <v>192</v>
       </c>
       <c r="C196" s="53" t="s">
-        <v>213</v>
-      </c>
-      <c r="D196" s="62"/>
+        <v>211</v>
+      </c>
+      <c r="D196" s="87"/>
       <c r="E196" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F196" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I196" s="99"/>
-      <c r="J196" s="99"/>
-      <c r="K196" s="100"/>
-      <c r="L196" s="99"/>
-      <c r="M196" s="99"/>
+      <c r="I196" s="27"/>
+      <c r="J196" s="27"/>
+      <c r="K196" s="84"/>
+      <c r="L196" s="27"/>
+      <c r="M196" s="27"/>
     </row>
     <row r="197" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B197" s="4">
@@ -4750,28 +4757,28 @@
       <c r="C197" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="D197" s="62"/>
+      <c r="D197" s="87"/>
       <c r="E197" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F197" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I197" s="99"/>
-      <c r="J197" s="99"/>
-      <c r="K197" s="100"/>
-      <c r="L197" s="99"/>
-      <c r="M197" s="99"/>
+      <c r="I197" s="27"/>
+      <c r="J197" s="27"/>
+      <c r="K197" s="84"/>
+      <c r="L197" s="27"/>
+      <c r="M197" s="27"/>
     </row>
     <row r="198" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B198" s="4">
         <v>194</v>
       </c>
       <c r="C198" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="D198" s="82" t="s">
         <v>214</v>
-      </c>
-      <c r="D198" s="59" t="s">
-        <v>216</v>
       </c>
       <c r="E198" s="54" t="s">
         <v>23</v>
@@ -4779,91 +4786,91 @@
       <c r="F198" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="I198" s="99"/>
-      <c r="J198" s="99"/>
-      <c r="K198" s="100"/>
-      <c r="L198" s="99"/>
-      <c r="M198" s="99"/>
+      <c r="I198" s="27"/>
+      <c r="J198" s="27"/>
+      <c r="K198" s="84"/>
+      <c r="L198" s="27"/>
+      <c r="M198" s="27"/>
     </row>
     <row r="199" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B199" s="4">
         <v>195</v>
       </c>
       <c r="C199" s="57" t="s">
-        <v>215</v>
-      </c>
-      <c r="D199" s="60"/>
+        <v>213</v>
+      </c>
+      <c r="D199" s="83"/>
       <c r="E199" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F199" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I199" s="99"/>
-      <c r="J199" s="99"/>
-      <c r="K199" s="100"/>
-      <c r="L199" s="99"/>
-      <c r="M199" s="99"/>
+      <c r="I199" s="27"/>
+      <c r="J199" s="27"/>
+      <c r="K199" s="84"/>
+      <c r="L199" s="27"/>
+      <c r="M199" s="27"/>
     </row>
     <row r="200" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B200" s="7">
         <v>196</v>
       </c>
       <c r="C200" s="57" t="s">
-        <v>218</v>
-      </c>
-      <c r="D200" s="60"/>
+        <v>216</v>
+      </c>
+      <c r="D200" s="83"/>
       <c r="E200" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F200" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I200" s="99"/>
-      <c r="J200" s="99"/>
-      <c r="K200" s="100"/>
-      <c r="L200" s="99"/>
-      <c r="M200" s="99"/>
+      <c r="I200" s="27"/>
+      <c r="J200" s="27"/>
+      <c r="K200" s="84"/>
+      <c r="L200" s="27"/>
+      <c r="M200" s="27"/>
     </row>
     <row r="201" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="4">
         <v>197</v>
       </c>
       <c r="C201" s="57" t="s">
-        <v>219</v>
-      </c>
-      <c r="D201" s="60"/>
+        <v>217</v>
+      </c>
+      <c r="D201" s="83"/>
       <c r="E201" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F201" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I201" s="99"/>
-      <c r="J201" s="99"/>
-      <c r="K201" s="100"/>
-      <c r="L201" s="99"/>
-      <c r="M201" s="99"/>
+      <c r="I201" s="27"/>
+      <c r="J201" s="27"/>
+      <c r="K201" s="84"/>
+      <c r="L201" s="27"/>
+      <c r="M201" s="27"/>
     </row>
     <row r="202" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B202" s="45">
         <v>198</v>
       </c>
       <c r="C202" s="58" t="s">
-        <v>220</v>
-      </c>
-      <c r="D202" s="60"/>
+        <v>218</v>
+      </c>
+      <c r="D202" s="83"/>
       <c r="E202" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F202" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I202" s="99"/>
-      <c r="J202" s="99"/>
-      <c r="K202" s="100"/>
-      <c r="L202" s="99"/>
-      <c r="M202" s="99"/>
+      <c r="I202" s="27"/>
+      <c r="J202" s="27"/>
+      <c r="K202" s="84"/>
+      <c r="L202" s="27"/>
+      <c r="M202" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:F202" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -4874,14 +4881,6 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="24">
-    <mergeCell ref="D83:D100"/>
-    <mergeCell ref="D101:D123"/>
-    <mergeCell ref="D124:D134"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="D17:D36"/>
     <mergeCell ref="D198:D202"/>
     <mergeCell ref="K186:K197"/>
     <mergeCell ref="K198:K202"/>
@@ -4898,6 +4897,14 @@
     <mergeCell ref="D159:D162"/>
     <mergeCell ref="D37:D49"/>
     <mergeCell ref="D50:D82"/>
+    <mergeCell ref="D83:D100"/>
+    <mergeCell ref="D101:D123"/>
+    <mergeCell ref="D124:D134"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="D17:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Nuevas funcionalidades parte 3
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/Requerimientos.xlsx
+++ b/DOCUMENTACION/Requerimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\grupo_tdm\grupotdm_admin\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C5C33-34BC-4B05-8B25-962371870DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D1D777-D970-4BEC-AF9E-5E934E4D0EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-510" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="222">
   <si>
     <t>REQUERIMIENTOS</t>
   </si>
@@ -669,9 +669,6 @@
     <t>El sistema debe validar la duplicidad de servidores por medio de la IP</t>
   </si>
   <si>
-    <t>El usuario desea editar el nombre, usuario y archivo de una llave VPN.</t>
-  </si>
-  <si>
     <t xml:space="preserve">NO </t>
   </si>
   <si>
@@ -703,6 +700,12 @@
   </si>
   <si>
     <t xml:space="preserve">El usuario desea editar el nombre MV, OS, servicio, observaciones, RAM, Vcpumu, TOTALDD,, SPLA RDP-TS y SPLA EXCEL de un servicor </t>
+  </si>
+  <si>
+    <t>El usuario desea editar el usuario y archivo de una llave VPN.</t>
+  </si>
+  <si>
+    <t>S I</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1190,6 +1193,63 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1256,61 +1316,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1630,8 +1636,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B3:M202"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="H182" sqref="H182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1646,18 +1652,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1688,7 +1694,7 @@
       <c r="C5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="89" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1705,7 +1711,7 @@
       <c r="C6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="71"/>
+      <c r="D6" s="90"/>
       <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1720,7 +1726,7 @@
       <c r="C7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="72"/>
+      <c r="D7" s="91"/>
       <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1735,7 +1741,7 @@
       <c r="C8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="92" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1752,7 +1758,7 @@
       <c r="C9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="74"/>
+      <c r="D9" s="93"/>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1767,7 +1773,7 @@
       <c r="C10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="74"/>
+      <c r="D10" s="93"/>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1782,7 +1788,7 @@
       <c r="C11" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="75"/>
+      <c r="D11" s="94"/>
       <c r="E11" s="9" t="s">
         <v>23</v>
       </c>
@@ -1797,7 +1803,7 @@
       <c r="C12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="95" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -1814,7 +1820,7 @@
       <c r="C13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="77"/>
+      <c r="D13" s="96"/>
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1829,7 +1835,7 @@
       <c r="C14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="77"/>
+      <c r="D14" s="96"/>
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1844,7 +1850,7 @@
       <c r="C15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="77"/>
+      <c r="D15" s="96"/>
       <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1859,7 +1865,7 @@
       <c r="C16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="78"/>
+      <c r="D16" s="97"/>
       <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
@@ -1874,7 +1880,7 @@
       <c r="C17" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="79" t="s">
+      <c r="D17" s="98" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1891,7 +1897,7 @@
       <c r="C18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="80"/>
+      <c r="D18" s="99"/>
       <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1906,7 +1912,7 @@
       <c r="C19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="80"/>
+      <c r="D19" s="99"/>
       <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1921,7 +1927,7 @@
       <c r="C20" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="80"/>
+      <c r="D20" s="99"/>
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1936,7 +1942,7 @@
       <c r="C21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="80"/>
+      <c r="D21" s="99"/>
       <c r="E21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1951,7 +1957,7 @@
       <c r="C22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="80"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1966,7 +1972,7 @@
       <c r="C23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="80"/>
+      <c r="D23" s="99"/>
       <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1981,7 +1987,7 @@
       <c r="C24" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="D24" s="80"/>
+      <c r="D24" s="99"/>
       <c r="E24" s="27" t="s">
         <v>23</v>
       </c>
@@ -1999,9 +2005,9 @@
         <v>21</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="D25" s="80"/>
+        <v>214</v>
+      </c>
+      <c r="D25" s="99"/>
       <c r="E25" s="27" t="s">
         <v>23</v>
       </c>
@@ -2021,7 +2027,7 @@
       <c r="C26" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="80"/>
+      <c r="D26" s="99"/>
       <c r="E26" s="27" t="s">
         <v>23</v>
       </c>
@@ -2041,7 +2047,7 @@
       <c r="C27" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="80"/>
+      <c r="D27" s="99"/>
       <c r="E27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2056,7 +2062,7 @@
       <c r="C28" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="80"/>
+      <c r="D28" s="99"/>
       <c r="E28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2071,7 +2077,7 @@
       <c r="C29" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="80"/>
+      <c r="D29" s="99"/>
       <c r="E29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2086,7 +2092,7 @@
       <c r="C30" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="80"/>
+      <c r="D30" s="99"/>
       <c r="E30" s="1" t="s">
         <v>23</v>
       </c>
@@ -2101,7 +2107,7 @@
       <c r="C31" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="80"/>
+      <c r="D31" s="99"/>
       <c r="E31" s="1" t="s">
         <v>23</v>
       </c>
@@ -2116,7 +2122,7 @@
       <c r="C32" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="80"/>
+      <c r="D32" s="99"/>
       <c r="E32" s="1" t="s">
         <v>23</v>
       </c>
@@ -2131,7 +2137,7 @@
       <c r="C33" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="80"/>
+      <c r="D33" s="99"/>
       <c r="E33" s="1" t="s">
         <v>23</v>
       </c>
@@ -2146,7 +2152,7 @@
       <c r="C34" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="80"/>
+      <c r="D34" s="99"/>
       <c r="E34" s="1" t="s">
         <v>23</v>
       </c>
@@ -2161,7 +2167,7 @@
       <c r="C35" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="80"/>
+      <c r="D35" s="99"/>
       <c r="E35" s="1" t="s">
         <v>23</v>
       </c>
@@ -2176,7 +2182,7 @@
       <c r="C36" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="81"/>
+      <c r="D36" s="100"/>
       <c r="E36" s="9" t="s">
         <v>23</v>
       </c>
@@ -2191,7 +2197,7 @@
       <c r="C37" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="95" t="s">
+      <c r="D37" s="74" t="s">
         <v>54</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -2208,7 +2214,7 @@
       <c r="C38" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="96"/>
+      <c r="D38" s="75"/>
       <c r="E38" s="1" t="s">
         <v>23</v>
       </c>
@@ -2223,7 +2229,7 @@
       <c r="C39" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="96"/>
+      <c r="D39" s="75"/>
       <c r="E39" s="1" t="s">
         <v>23</v>
       </c>
@@ -2238,7 +2244,7 @@
       <c r="C40" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="96"/>
+      <c r="D40" s="75"/>
       <c r="E40" s="1" t="s">
         <v>23</v>
       </c>
@@ -2253,7 +2259,7 @@
       <c r="C41" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="96"/>
+      <c r="D41" s="75"/>
       <c r="E41" s="1" t="s">
         <v>23</v>
       </c>
@@ -2268,7 +2274,7 @@
       <c r="C42" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="96"/>
+      <c r="D42" s="75"/>
       <c r="E42" s="1" t="s">
         <v>23</v>
       </c>
@@ -2283,7 +2289,7 @@
       <c r="C43" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="96"/>
+      <c r="D43" s="75"/>
       <c r="E43" s="1" t="s">
         <v>23</v>
       </c>
@@ -2298,7 +2304,7 @@
       <c r="C44" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="96"/>
+      <c r="D44" s="75"/>
       <c r="E44" s="1" t="s">
         <v>23</v>
       </c>
@@ -2313,7 +2319,7 @@
       <c r="C45" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="96"/>
+      <c r="D45" s="75"/>
       <c r="F45" s="8" t="s">
         <v>23</v>
       </c>
@@ -2325,7 +2331,7 @@
       <c r="C46" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="96"/>
+      <c r="D46" s="75"/>
       <c r="E46" s="1" t="s">
         <v>23</v>
       </c>
@@ -2340,7 +2346,7 @@
       <c r="C47" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="96"/>
+      <c r="D47" s="75"/>
       <c r="E47" s="1" t="s">
         <v>23</v>
       </c>
@@ -2355,7 +2361,7 @@
       <c r="C48" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="96"/>
+      <c r="D48" s="75"/>
       <c r="E48" s="1" t="s">
         <v>23</v>
       </c>
@@ -2370,7 +2376,7 @@
       <c r="C49" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="96"/>
+      <c r="D49" s="75"/>
       <c r="E49" s="1" t="s">
         <v>23</v>
       </c>
@@ -2385,7 +2391,7 @@
       <c r="C50" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="97" t="s">
+      <c r="D50" s="76" t="s">
         <v>83</v>
       </c>
       <c r="E50" s="5" t="s">
@@ -2402,7 +2408,7 @@
       <c r="C51" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="98"/>
+      <c r="D51" s="77"/>
       <c r="E51" s="1" t="s">
         <v>23</v>
       </c>
@@ -2417,7 +2423,7 @@
       <c r="C52" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D52" s="98"/>
+      <c r="D52" s="77"/>
       <c r="E52" s="1" t="s">
         <v>23</v>
       </c>
@@ -2432,7 +2438,7 @@
       <c r="C53" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D53" s="98"/>
+      <c r="D53" s="77"/>
       <c r="F53" s="8"/>
     </row>
     <row r="54" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2442,7 +2448,7 @@
       <c r="C54" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="98"/>
+      <c r="D54" s="77"/>
       <c r="E54" s="1" t="s">
         <v>23</v>
       </c>
@@ -2457,7 +2463,7 @@
       <c r="C55" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="98"/>
+      <c r="D55" s="77"/>
       <c r="E55" s="1" t="s">
         <v>23</v>
       </c>
@@ -2472,7 +2478,7 @@
       <c r="C56" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="98"/>
+      <c r="D56" s="77"/>
       <c r="E56" s="1" t="s">
         <v>23</v>
       </c>
@@ -2487,7 +2493,7 @@
       <c r="C57" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="98"/>
+      <c r="D57" s="77"/>
       <c r="E57" s="1" t="s">
         <v>23</v>
       </c>
@@ -2502,7 +2508,7 @@
       <c r="C58" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="98"/>
+      <c r="D58" s="77"/>
       <c r="E58" s="1" t="s">
         <v>23</v>
       </c>
@@ -2517,7 +2523,7 @@
       <c r="C59" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="98"/>
+      <c r="D59" s="77"/>
       <c r="E59" s="1" t="s">
         <v>23</v>
       </c>
@@ -2532,7 +2538,7 @@
       <c r="C60" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D60" s="98"/>
+      <c r="D60" s="77"/>
       <c r="E60" s="1" t="s">
         <v>23</v>
       </c>
@@ -2547,7 +2553,7 @@
       <c r="C61" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="98"/>
+      <c r="D61" s="77"/>
       <c r="E61" s="1" t="s">
         <v>23</v>
       </c>
@@ -2562,7 +2568,7 @@
       <c r="C62" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="98"/>
+      <c r="D62" s="77"/>
       <c r="E62" s="1" t="s">
         <v>23</v>
       </c>
@@ -2577,7 +2583,7 @@
       <c r="C63" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="98"/>
+      <c r="D63" s="77"/>
       <c r="E63" s="1" t="s">
         <v>23</v>
       </c>
@@ -2592,7 +2598,7 @@
       <c r="C64" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D64" s="98"/>
+      <c r="D64" s="77"/>
       <c r="E64" s="1" t="s">
         <v>23</v>
       </c>
@@ -2607,7 +2613,7 @@
       <c r="C65" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="98"/>
+      <c r="D65" s="77"/>
       <c r="E65" s="1" t="s">
         <v>23</v>
       </c>
@@ -2622,7 +2628,7 @@
       <c r="C66" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="98"/>
+      <c r="D66" s="77"/>
       <c r="E66" s="1" t="s">
         <v>23</v>
       </c>
@@ -2637,7 +2643,7 @@
       <c r="C67" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D67" s="98"/>
+      <c r="D67" s="77"/>
       <c r="E67" s="1" t="s">
         <v>23</v>
       </c>
@@ -2652,7 +2658,7 @@
       <c r="C68" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="98"/>
+      <c r="D68" s="77"/>
       <c r="E68" s="1" t="s">
         <v>23</v>
       </c>
@@ -2667,7 +2673,7 @@
       <c r="C69" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D69" s="98"/>
+      <c r="D69" s="77"/>
       <c r="E69" s="1" t="s">
         <v>23</v>
       </c>
@@ -2682,7 +2688,7 @@
       <c r="C70" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="D70" s="98"/>
+      <c r="D70" s="77"/>
       <c r="F70" s="8"/>
     </row>
     <row r="71" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
@@ -2692,7 +2698,7 @@
       <c r="C71" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="D71" s="98"/>
+      <c r="D71" s="77"/>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2702,7 +2708,7 @@
       <c r="C72" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="98"/>
+      <c r="D72" s="77"/>
       <c r="E72" s="1" t="s">
         <v>23</v>
       </c>
@@ -2717,7 +2723,7 @@
       <c r="C73" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D73" s="98"/>
+      <c r="D73" s="77"/>
       <c r="E73" s="1" t="s">
         <v>23</v>
       </c>
@@ -2732,7 +2738,7 @@
       <c r="C74" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="98"/>
+      <c r="D74" s="77"/>
       <c r="E74" s="1" t="s">
         <v>23</v>
       </c>
@@ -2747,7 +2753,7 @@
       <c r="C75" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D75" s="98"/>
+      <c r="D75" s="77"/>
       <c r="E75" s="1" t="s">
         <v>23</v>
       </c>
@@ -2762,7 +2768,7 @@
       <c r="C76" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="98"/>
+      <c r="D76" s="77"/>
       <c r="E76" s="1" t="s">
         <v>23</v>
       </c>
@@ -2777,7 +2783,7 @@
       <c r="C77" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D77" s="98"/>
+      <c r="D77" s="77"/>
       <c r="E77" s="1" t="s">
         <v>23</v>
       </c>
@@ -2792,7 +2798,7 @@
       <c r="C78" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D78" s="98"/>
+      <c r="D78" s="77"/>
       <c r="E78" s="1" t="s">
         <v>23</v>
       </c>
@@ -2807,7 +2813,7 @@
       <c r="C79" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D79" s="98"/>
+      <c r="D79" s="77"/>
       <c r="E79" s="1" t="s">
         <v>23</v>
       </c>
@@ -2822,7 +2828,7 @@
       <c r="C80" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D80" s="98"/>
+      <c r="D80" s="77"/>
       <c r="F80" s="8"/>
     </row>
     <row r="81" spans="2:6" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
@@ -2832,7 +2838,7 @@
       <c r="C81" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D81" s="98"/>
+      <c r="D81" s="77"/>
       <c r="F81" s="8"/>
     </row>
     <row r="82" spans="2:6" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2842,7 +2848,7 @@
       <c r="C82" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="99"/>
+      <c r="D82" s="78"/>
       <c r="E82" s="9" t="s">
         <v>23</v>
       </c>
@@ -2857,7 +2863,7 @@
       <c r="C83" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D83" s="60" t="s">
+      <c r="D83" s="79" t="s">
         <v>103</v>
       </c>
       <c r="E83" s="5" t="s">
@@ -2874,7 +2880,7 @@
       <c r="C84" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D84" s="61"/>
+      <c r="D84" s="80"/>
       <c r="E84" s="1" t="s">
         <v>23</v>
       </c>
@@ -2889,7 +2895,7 @@
       <c r="C85" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D85" s="61"/>
+      <c r="D85" s="80"/>
       <c r="E85" s="1" t="s">
         <v>23</v>
       </c>
@@ -2904,7 +2910,7 @@
       <c r="C86" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D86" s="61"/>
+      <c r="D86" s="80"/>
       <c r="E86" s="1" t="s">
         <v>23</v>
       </c>
@@ -2919,7 +2925,7 @@
       <c r="C87" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D87" s="61"/>
+      <c r="D87" s="80"/>
       <c r="E87" s="1" t="s">
         <v>23</v>
       </c>
@@ -2934,7 +2940,7 @@
       <c r="C88" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D88" s="61"/>
+      <c r="D88" s="80"/>
       <c r="E88" s="1" t="s">
         <v>23</v>
       </c>
@@ -2949,7 +2955,7 @@
       <c r="C89" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D89" s="61"/>
+      <c r="D89" s="80"/>
       <c r="E89" s="1" t="s">
         <v>23</v>
       </c>
@@ -2964,7 +2970,7 @@
       <c r="C90" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D90" s="61"/>
+      <c r="D90" s="80"/>
       <c r="E90" s="1" t="s">
         <v>23</v>
       </c>
@@ -2979,7 +2985,7 @@
       <c r="C91" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D91" s="61"/>
+      <c r="D91" s="80"/>
       <c r="E91" s="1" t="s">
         <v>23</v>
       </c>
@@ -2994,7 +3000,7 @@
       <c r="C92" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D92" s="61"/>
+      <c r="D92" s="80"/>
       <c r="E92" s="1" t="s">
         <v>23</v>
       </c>
@@ -3009,7 +3015,7 @@
       <c r="C93" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D93" s="61"/>
+      <c r="D93" s="80"/>
       <c r="E93" s="1" t="s">
         <v>23</v>
       </c>
@@ -3024,7 +3030,7 @@
       <c r="C94" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D94" s="61"/>
+      <c r="D94" s="80"/>
       <c r="E94" s="1" t="s">
         <v>23</v>
       </c>
@@ -3039,7 +3045,7 @@
       <c r="C95" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D95" s="61"/>
+      <c r="D95" s="80"/>
       <c r="E95" s="1" t="s">
         <v>23</v>
       </c>
@@ -3054,7 +3060,7 @@
       <c r="C96" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D96" s="61"/>
+      <c r="D96" s="80"/>
       <c r="E96" s="1" t="s">
         <v>23</v>
       </c>
@@ -3069,7 +3075,7 @@
       <c r="C97" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D97" s="61"/>
+      <c r="D97" s="80"/>
       <c r="E97" s="1" t="s">
         <v>23</v>
       </c>
@@ -3084,7 +3090,7 @@
       <c r="C98" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D98" s="61"/>
+      <c r="D98" s="80"/>
       <c r="E98" s="1" t="s">
         <v>23</v>
       </c>
@@ -3099,7 +3105,7 @@
       <c r="C99" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D99" s="61"/>
+      <c r="D99" s="80"/>
       <c r="E99" s="1" t="s">
         <v>23</v>
       </c>
@@ -3114,7 +3120,7 @@
       <c r="C100" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D100" s="62"/>
+      <c r="D100" s="81"/>
       <c r="E100" s="9" t="s">
         <v>23</v>
       </c>
@@ -3129,7 +3135,7 @@
       <c r="C101" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D101" s="63" t="s">
+      <c r="D101" s="82" t="s">
         <v>126</v>
       </c>
       <c r="E101" s="5" t="s">
@@ -3146,7 +3152,7 @@
       <c r="C102" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D102" s="64"/>
+      <c r="D102" s="83"/>
       <c r="E102" s="1" t="s">
         <v>23</v>
       </c>
@@ -3161,7 +3167,7 @@
       <c r="C103" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D103" s="64"/>
+      <c r="D103" s="83"/>
       <c r="E103" s="1" t="s">
         <v>23</v>
       </c>
@@ -3176,7 +3182,7 @@
       <c r="C104" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D104" s="64"/>
+      <c r="D104" s="83"/>
       <c r="E104" s="1" t="s">
         <v>23</v>
       </c>
@@ -3191,7 +3197,7 @@
       <c r="C105" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D105" s="64"/>
+      <c r="D105" s="83"/>
       <c r="E105" s="1" t="s">
         <v>23</v>
       </c>
@@ -3206,7 +3212,7 @@
       <c r="C106" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D106" s="64"/>
+      <c r="D106" s="83"/>
       <c r="E106" s="1" t="s">
         <v>23</v>
       </c>
@@ -3221,7 +3227,7 @@
       <c r="C107" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D107" s="64"/>
+      <c r="D107" s="83"/>
       <c r="E107" s="1" t="s">
         <v>23</v>
       </c>
@@ -3236,7 +3242,7 @@
       <c r="C108" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D108" s="64"/>
+      <c r="D108" s="83"/>
       <c r="E108" s="1" t="s">
         <v>23</v>
       </c>
@@ -3251,7 +3257,7 @@
       <c r="C109" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D109" s="64"/>
+      <c r="D109" s="83"/>
       <c r="E109" s="1" t="s">
         <v>23</v>
       </c>
@@ -3266,7 +3272,7 @@
       <c r="C110" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D110" s="64"/>
+      <c r="D110" s="83"/>
       <c r="E110" s="1" t="s">
         <v>23</v>
       </c>
@@ -3281,7 +3287,7 @@
       <c r="C111" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D111" s="64"/>
+      <c r="D111" s="83"/>
       <c r="E111" s="1" t="s">
         <v>23</v>
       </c>
@@ -3296,7 +3302,7 @@
       <c r="C112" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="D112" s="64"/>
+      <c r="D112" s="83"/>
       <c r="E112" s="1" t="s">
         <v>23</v>
       </c>
@@ -3311,7 +3317,7 @@
       <c r="C113" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D113" s="64"/>
+      <c r="D113" s="83"/>
       <c r="E113" s="1" t="s">
         <v>23</v>
       </c>
@@ -3326,7 +3332,7 @@
       <c r="C114" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D114" s="64"/>
+      <c r="D114" s="83"/>
       <c r="E114" s="1" t="s">
         <v>23</v>
       </c>
@@ -3341,7 +3347,7 @@
       <c r="C115" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="D115" s="64"/>
+      <c r="D115" s="83"/>
       <c r="E115" s="1" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3362,7 @@
       <c r="C116" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D116" s="64"/>
+      <c r="D116" s="83"/>
       <c r="E116" s="1" t="s">
         <v>23</v>
       </c>
@@ -3371,7 +3377,7 @@
       <c r="C117" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D117" s="64"/>
+      <c r="D117" s="83"/>
       <c r="E117" s="1" t="s">
         <v>23</v>
       </c>
@@ -3386,7 +3392,7 @@
       <c r="C118" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D118" s="64"/>
+      <c r="D118" s="83"/>
       <c r="E118" s="1" t="s">
         <v>23</v>
       </c>
@@ -3401,7 +3407,7 @@
       <c r="C119" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D119" s="64"/>
+      <c r="D119" s="83"/>
       <c r="E119" s="1" t="s">
         <v>23</v>
       </c>
@@ -3416,7 +3422,7 @@
       <c r="C120" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D120" s="64"/>
+      <c r="D120" s="83"/>
       <c r="E120" s="1" t="s">
         <v>23</v>
       </c>
@@ -3431,7 +3437,7 @@
       <c r="C121" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D121" s="64"/>
+      <c r="D121" s="83"/>
       <c r="E121" s="1" t="s">
         <v>23</v>
       </c>
@@ -3446,7 +3452,7 @@
       <c r="C122" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D122" s="64"/>
+      <c r="D122" s="83"/>
       <c r="E122" s="1" t="s">
         <v>23</v>
       </c>
@@ -3461,7 +3467,7 @@
       <c r="C123" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D123" s="65"/>
+      <c r="D123" s="84"/>
       <c r="E123" s="9" t="s">
         <v>23</v>
       </c>
@@ -3476,7 +3482,7 @@
       <c r="C124" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D124" s="66" t="s">
+      <c r="D124" s="85" t="s">
         <v>140</v>
       </c>
       <c r="E124" s="5" t="s">
@@ -3493,7 +3499,7 @@
       <c r="C125" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="D125" s="67"/>
+      <c r="D125" s="86"/>
       <c r="E125" s="1" t="s">
         <v>23</v>
       </c>
@@ -3508,7 +3514,7 @@
       <c r="C126" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="D126" s="67"/>
+      <c r="D126" s="86"/>
       <c r="E126" s="1" t="s">
         <v>23</v>
       </c>
@@ -3523,7 +3529,7 @@
       <c r="C127" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D127" s="67"/>
+      <c r="D127" s="86"/>
       <c r="E127" s="1" t="s">
         <v>23</v>
       </c>
@@ -3538,7 +3544,7 @@
       <c r="C128" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D128" s="67"/>
+      <c r="D128" s="86"/>
       <c r="E128" s="1" t="s">
         <v>23</v>
       </c>
@@ -3553,7 +3559,7 @@
       <c r="C129" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D129" s="67"/>
+      <c r="D129" s="86"/>
       <c r="E129" s="1" t="s">
         <v>23</v>
       </c>
@@ -3568,7 +3574,7 @@
       <c r="C130" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="D130" s="67"/>
+      <c r="D130" s="86"/>
       <c r="E130" s="1" t="s">
         <v>23</v>
       </c>
@@ -3583,7 +3589,7 @@
       <c r="C131" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D131" s="67"/>
+      <c r="D131" s="86"/>
       <c r="E131" s="1" t="s">
         <v>23</v>
       </c>
@@ -3598,7 +3604,7 @@
       <c r="C132" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D132" s="67"/>
+      <c r="D132" s="86"/>
       <c r="E132" s="1" t="s">
         <v>23</v>
       </c>
@@ -3613,7 +3619,7 @@
       <c r="C133" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="D133" s="67"/>
+      <c r="D133" s="86"/>
       <c r="E133" s="1" t="s">
         <v>23</v>
       </c>
@@ -3628,7 +3634,7 @@
       <c r="C134" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D134" s="68"/>
+      <c r="D134" s="87"/>
       <c r="E134" s="9" t="s">
         <v>23</v>
       </c>
@@ -3643,7 +3649,7 @@
       <c r="C135" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D135" s="88" t="s">
+      <c r="D135" s="67" t="s">
         <v>164</v>
       </c>
       <c r="E135" s="5" t="s">
@@ -3660,7 +3666,7 @@
       <c r="C136" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D136" s="89"/>
+      <c r="D136" s="68"/>
       <c r="E136" s="1" t="s">
         <v>23</v>
       </c>
@@ -3675,7 +3681,7 @@
       <c r="C137" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D137" s="89"/>
+      <c r="D137" s="68"/>
       <c r="E137" s="1" t="s">
         <v>23</v>
       </c>
@@ -3690,7 +3696,7 @@
       <c r="C138" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D138" s="89"/>
+      <c r="D138" s="68"/>
       <c r="E138" s="1" t="s">
         <v>23</v>
       </c>
@@ -3705,7 +3711,7 @@
       <c r="C139" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="D139" s="89"/>
+      <c r="D139" s="68"/>
       <c r="E139" s="1" t="s">
         <v>23</v>
       </c>
@@ -3720,7 +3726,7 @@
       <c r="C140" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D140" s="89"/>
+      <c r="D140" s="68"/>
       <c r="E140" s="1" t="s">
         <v>23</v>
       </c>
@@ -3735,7 +3741,7 @@
       <c r="C141" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D141" s="89"/>
+      <c r="D141" s="68"/>
       <c r="E141" s="1" t="s">
         <v>23</v>
       </c>
@@ -3750,7 +3756,7 @@
       <c r="C142" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D142" s="89"/>
+      <c r="D142" s="68"/>
       <c r="E142" s="1" t="s">
         <v>23</v>
       </c>
@@ -3765,7 +3771,7 @@
       <c r="C143" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D143" s="89"/>
+      <c r="D143" s="68"/>
       <c r="E143" s="1" t="s">
         <v>23</v>
       </c>
@@ -3780,7 +3786,7 @@
       <c r="C144" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D144" s="89"/>
+      <c r="D144" s="68"/>
       <c r="E144" s="1" t="s">
         <v>23</v>
       </c>
@@ -3795,7 +3801,7 @@
       <c r="C145" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="D145" s="89"/>
+      <c r="D145" s="68"/>
       <c r="E145" s="1" t="s">
         <v>23</v>
       </c>
@@ -3810,7 +3816,7 @@
       <c r="C146" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D146" s="89"/>
+      <c r="D146" s="68"/>
       <c r="E146" s="1" t="s">
         <v>23</v>
       </c>
@@ -3825,7 +3831,7 @@
       <c r="C147" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D147" s="89"/>
+      <c r="D147" s="68"/>
       <c r="E147" s="1" t="s">
         <v>23</v>
       </c>
@@ -3840,7 +3846,7 @@
       <c r="C148" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="D148" s="89"/>
+      <c r="D148" s="68"/>
       <c r="E148" s="1" t="s">
         <v>23</v>
       </c>
@@ -3855,7 +3861,7 @@
       <c r="C149" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D149" s="89"/>
+      <c r="D149" s="68"/>
       <c r="E149" s="1" t="s">
         <v>23</v>
       </c>
@@ -3870,7 +3876,7 @@
       <c r="C150" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D150" s="89"/>
+      <c r="D150" s="68"/>
       <c r="E150" s="1" t="s">
         <v>23</v>
       </c>
@@ -3885,7 +3891,7 @@
       <c r="C151" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D151" s="89"/>
+      <c r="D151" s="68"/>
       <c r="E151" s="1" t="s">
         <v>23</v>
       </c>
@@ -3900,7 +3906,7 @@
       <c r="C152" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D152" s="89"/>
+      <c r="D152" s="68"/>
       <c r="E152" s="1" t="s">
         <v>23</v>
       </c>
@@ -3915,7 +3921,7 @@
       <c r="C153" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D153" s="89"/>
+      <c r="D153" s="68"/>
       <c r="E153" s="1" t="s">
         <v>23</v>
       </c>
@@ -3930,7 +3936,7 @@
       <c r="C154" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D154" s="89"/>
+      <c r="D154" s="68"/>
       <c r="E154" s="1" t="s">
         <v>23</v>
       </c>
@@ -3945,7 +3951,7 @@
       <c r="C155" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D155" s="89"/>
+      <c r="D155" s="68"/>
       <c r="E155" s="1" t="s">
         <v>23</v>
       </c>
@@ -3960,7 +3966,7 @@
       <c r="C156" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D156" s="90"/>
+      <c r="D156" s="69"/>
       <c r="E156" s="9" t="s">
         <v>23</v>
       </c>
@@ -3975,7 +3981,7 @@
       <c r="C157" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D157" s="91" t="s">
+      <c r="D157" s="70" t="s">
         <v>167</v>
       </c>
       <c r="E157" s="5" t="s">
@@ -3992,7 +3998,7 @@
       <c r="C158" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D158" s="92"/>
+      <c r="D158" s="71"/>
       <c r="E158" s="9" t="s">
         <v>23</v>
       </c>
@@ -4007,7 +4013,7 @@
       <c r="C159" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="D159" s="93" t="s">
+      <c r="D159" s="72" t="s">
         <v>172</v>
       </c>
       <c r="E159" s="5" t="s">
@@ -4024,7 +4030,7 @@
       <c r="C160" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="D160" s="94"/>
+      <c r="D160" s="73"/>
       <c r="E160" s="1" t="s">
         <v>23</v>
       </c>
@@ -4039,7 +4045,7 @@
       <c r="C161" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D161" s="94"/>
+      <c r="D161" s="73"/>
       <c r="E161" s="1" t="s">
         <v>23</v>
       </c>
@@ -4054,7 +4060,7 @@
       <c r="C162" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D162" s="94"/>
+      <c r="D162" s="73"/>
       <c r="E162" s="1" t="s">
         <v>23</v>
       </c>
@@ -4069,7 +4075,7 @@
       <c r="C163" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="D163" s="86" t="s">
+      <c r="D163" s="65" t="s">
         <v>177</v>
       </c>
       <c r="E163" s="5" t="s">
@@ -4080,7 +4086,7 @@
       </c>
       <c r="I163" s="27"/>
       <c r="J163" s="27"/>
-      <c r="K163" s="84"/>
+      <c r="K163" s="63"/>
       <c r="L163" s="27"/>
       <c r="M163" s="27"/>
     </row>
@@ -4091,7 +4097,7 @@
       <c r="C164" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="D164" s="87"/>
+      <c r="D164" s="66"/>
       <c r="E164" s="1" t="s">
         <v>23</v>
       </c>
@@ -4100,7 +4106,7 @@
       </c>
       <c r="I164" s="27"/>
       <c r="J164" s="27"/>
-      <c r="K164" s="84"/>
+      <c r="K164" s="63"/>
       <c r="L164" s="27"/>
       <c r="M164" s="27"/>
     </row>
@@ -4111,7 +4117,7 @@
       <c r="C165" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="D165" s="87"/>
+      <c r="D165" s="66"/>
       <c r="E165" s="1" t="s">
         <v>25</v>
       </c>
@@ -4120,47 +4126,47 @@
       </c>
       <c r="I165" s="27"/>
       <c r="J165" s="27"/>
-      <c r="K165" s="84"/>
+      <c r="K165" s="63"/>
       <c r="L165" s="27"/>
       <c r="M165" s="27"/>
     </row>
-    <row r="166" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B166" s="7">
         <v>162</v>
       </c>
       <c r="C166" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="D166" s="87"/>
+      <c r="D166" s="66"/>
       <c r="E166" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I166" s="27"/>
       <c r="J166" s="27"/>
-      <c r="K166" s="84"/>
+      <c r="K166" s="63"/>
       <c r="L166" s="27"/>
       <c r="M166" s="27"/>
     </row>
-    <row r="167" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B167" s="4">
         <v>163</v>
       </c>
       <c r="C167" s="44" t="s">
-        <v>219</v>
-      </c>
-      <c r="D167" s="87"/>
+        <v>218</v>
+      </c>
+      <c r="D167" s="66"/>
       <c r="E167" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I167" s="27"/>
       <c r="J167" s="27"/>
-      <c r="K167" s="84"/>
+      <c r="K167" s="63"/>
       <c r="L167" s="27"/>
       <c r="M167" s="27"/>
     </row>
@@ -4171,7 +4177,7 @@
       <c r="C168" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="D168" s="87"/>
+      <c r="D168" s="66"/>
       <c r="E168" s="1" t="s">
         <v>23</v>
       </c>
@@ -4180,7 +4186,7 @@
       </c>
       <c r="I168" s="27"/>
       <c r="J168" s="27"/>
-      <c r="K168" s="84"/>
+      <c r="K168" s="63"/>
       <c r="L168" s="27"/>
       <c r="M168" s="27"/>
     </row>
@@ -4188,10 +4194,10 @@
       <c r="B169" s="4">
         <v>165</v>
       </c>
-      <c r="C169" s="100" t="s">
+      <c r="C169" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="D169" s="87"/>
+      <c r="D169" s="66"/>
       <c r="E169" s="1" t="s">
         <v>23</v>
       </c>
@@ -4200,7 +4206,7 @@
       </c>
       <c r="I169" s="27"/>
       <c r="J169" s="27"/>
-      <c r="K169" s="84"/>
+      <c r="K169" s="63"/>
       <c r="L169" s="27"/>
       <c r="M169" s="27"/>
     </row>
@@ -4209,9 +4215,9 @@
         <v>166</v>
       </c>
       <c r="C170" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="D170" s="87"/>
+        <v>219</v>
+      </c>
+      <c r="D170" s="66"/>
       <c r="E170" s="1" t="s">
         <v>23</v>
       </c>
@@ -4220,7 +4226,7 @@
       </c>
       <c r="I170" s="27"/>
       <c r="J170" s="27"/>
-      <c r="K170" s="84"/>
+      <c r="K170" s="63"/>
       <c r="L170" s="27"/>
       <c r="M170" s="27"/>
     </row>
@@ -4231,7 +4237,7 @@
       <c r="C171" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="D171" s="87"/>
+      <c r="D171" s="66"/>
       <c r="E171" s="1" t="s">
         <v>23</v>
       </c>
@@ -4240,7 +4246,7 @@
       </c>
       <c r="I171" s="27"/>
       <c r="J171" s="27"/>
-      <c r="K171" s="84"/>
+      <c r="K171" s="63"/>
       <c r="L171" s="27"/>
       <c r="M171" s="27"/>
     </row>
@@ -4251,7 +4257,7 @@
       <c r="C172" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="D172" s="87"/>
+      <c r="D172" s="66"/>
       <c r="E172" s="1" t="s">
         <v>23</v>
       </c>
@@ -4260,7 +4266,7 @@
       </c>
       <c r="I172" s="27"/>
       <c r="J172" s="27"/>
-      <c r="K172" s="84"/>
+      <c r="K172" s="63"/>
       <c r="L172" s="27"/>
       <c r="M172" s="27"/>
     </row>
@@ -4271,7 +4277,7 @@
       <c r="C173" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="D173" s="87"/>
+      <c r="D173" s="66"/>
       <c r="E173" s="1" t="s">
         <v>23</v>
       </c>
@@ -4280,7 +4286,7 @@
       </c>
       <c r="I173" s="27"/>
       <c r="J173" s="27"/>
-      <c r="K173" s="84"/>
+      <c r="K173" s="63"/>
       <c r="L173" s="27"/>
       <c r="M173" s="27"/>
     </row>
@@ -4291,7 +4297,7 @@
       <c r="C174" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="D174" s="87"/>
+      <c r="D174" s="66"/>
       <c r="E174" s="1" t="s">
         <v>23</v>
       </c>
@@ -4300,7 +4306,7 @@
       </c>
       <c r="I174" s="27"/>
       <c r="J174" s="27"/>
-      <c r="K174" s="84"/>
+      <c r="K174" s="63"/>
       <c r="L174" s="27"/>
       <c r="M174" s="27"/>
     </row>
@@ -4311,7 +4317,7 @@
       <c r="C175" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="D175" s="83"/>
+      <c r="D175" s="62"/>
       <c r="E175" s="9" t="s">
         <v>23</v>
       </c>
@@ -4320,120 +4326,120 @@
       </c>
       <c r="I175" s="27"/>
       <c r="J175" s="27"/>
-      <c r="K175" s="84"/>
+      <c r="K175" s="63"/>
       <c r="L175" s="27"/>
       <c r="M175" s="27"/>
     </row>
-    <row r="176" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="7">
         <v>172</v>
       </c>
       <c r="C176" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="D176" s="86" t="s">
+      <c r="D176" s="65" t="s">
         <v>207</v>
       </c>
       <c r="E176" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F176" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I176" s="27"/>
       <c r="J176" s="27"/>
-      <c r="K176" s="84"/>
+      <c r="K176" s="63"/>
       <c r="L176" s="27"/>
       <c r="M176" s="27"/>
     </row>
-    <row r="177" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B177" s="4">
         <v>173</v>
       </c>
       <c r="C177" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="D177" s="87"/>
+      <c r="D177" s="66"/>
       <c r="E177" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I177" s="27"/>
       <c r="J177" s="27"/>
-      <c r="K177" s="84"/>
+      <c r="K177" s="63"/>
       <c r="L177" s="27"/>
       <c r="M177" s="27"/>
     </row>
-    <row r="178" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B178" s="7">
         <v>174</v>
       </c>
       <c r="C178" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="D178" s="87"/>
+      <c r="D178" s="66"/>
       <c r="E178" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I178" s="27"/>
       <c r="J178" s="27"/>
-      <c r="K178" s="84"/>
+      <c r="K178" s="63"/>
       <c r="L178" s="27"/>
       <c r="M178" s="27"/>
     </row>
-    <row r="179" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B179" s="4">
         <v>175</v>
       </c>
       <c r="C179" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="D179" s="87"/>
+      <c r="D179" s="66"/>
       <c r="E179" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I179" s="27"/>
       <c r="J179" s="27"/>
-      <c r="K179" s="84"/>
+      <c r="K179" s="63"/>
       <c r="L179" s="27"/>
       <c r="M179" s="27"/>
     </row>
-    <row r="180" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B180" s="7">
         <v>176</v>
       </c>
       <c r="C180" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="D180" s="83"/>
+      <c r="D180" s="62"/>
       <c r="E180" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F180" s="10" t="s">
-        <v>25</v>
+      <c r="F180" s="101" t="s">
+        <v>23</v>
       </c>
       <c r="I180" s="27"/>
       <c r="J180" s="27"/>
-      <c r="K180" s="84"/>
+      <c r="K180" s="63"/>
       <c r="L180" s="27"/>
       <c r="M180" s="27"/>
     </row>
-    <row r="181" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B181" s="4">
         <v>177</v>
       </c>
       <c r="C181" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="D181" s="86" t="s">
+      <c r="D181" s="65" t="s">
         <v>206</v>
       </c>
       <c r="E181" s="5" t="s">
@@ -4444,27 +4450,27 @@
       </c>
       <c r="I181" s="27"/>
       <c r="J181" s="27"/>
-      <c r="K181" s="84"/>
+      <c r="K181" s="63"/>
       <c r="L181" s="27"/>
       <c r="M181" s="27"/>
     </row>
-    <row r="182" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B182" s="7">
         <v>178</v>
       </c>
       <c r="C182" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="D182" s="87"/>
+      <c r="D182" s="66"/>
       <c r="E182" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I182" s="27"/>
       <c r="J182" s="27"/>
-      <c r="K182" s="84"/>
+      <c r="K182" s="63"/>
       <c r="L182" s="27"/>
       <c r="M182" s="27"/>
     </row>
@@ -4475,7 +4481,7 @@
       <c r="C183" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="D183" s="87"/>
+      <c r="D183" s="66"/>
       <c r="E183" s="1" t="s">
         <v>23</v>
       </c>
@@ -4484,7 +4490,7 @@
       </c>
       <c r="I183" s="27"/>
       <c r="J183" s="27"/>
-      <c r="K183" s="84"/>
+      <c r="K183" s="63"/>
       <c r="L183" s="27"/>
       <c r="M183" s="27"/>
     </row>
@@ -4495,7 +4501,7 @@
       <c r="C184" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="D184" s="87"/>
+      <c r="D184" s="66"/>
       <c r="E184" s="1" t="s">
         <v>23</v>
       </c>
@@ -4504,7 +4510,7 @@
       </c>
       <c r="I184" s="27"/>
       <c r="J184" s="27"/>
-      <c r="K184" s="84"/>
+      <c r="K184" s="63"/>
       <c r="L184" s="27"/>
       <c r="M184" s="27"/>
     </row>
@@ -4515,7 +4521,7 @@
       <c r="C185" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="D185" s="83"/>
+      <c r="D185" s="62"/>
       <c r="E185" s="9" t="s">
         <v>23</v>
       </c>
@@ -4524,120 +4530,120 @@
       </c>
       <c r="I185" s="27"/>
       <c r="J185" s="27"/>
-      <c r="K185" s="84"/>
+      <c r="K185" s="63"/>
       <c r="L185" s="27"/>
       <c r="M185" s="27"/>
     </row>
-    <row r="186" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B186" s="7">
         <v>182</v>
       </c>
       <c r="C186" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="D186" s="86" t="s">
+      <c r="D186" s="65" t="s">
         <v>178</v>
       </c>
       <c r="E186" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F186" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I186" s="27"/>
       <c r="J186" s="27"/>
-      <c r="K186" s="84"/>
+      <c r="K186" s="63"/>
       <c r="L186" s="27"/>
       <c r="M186" s="27"/>
     </row>
-    <row r="187" spans="2:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:13" ht="100.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B187" s="4">
         <v>183</v>
       </c>
       <c r="C187" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="D187" s="87"/>
+      <c r="D187" s="66"/>
       <c r="E187" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I187" s="27"/>
       <c r="J187" s="27"/>
-      <c r="K187" s="84"/>
+      <c r="K187" s="63"/>
       <c r="L187" s="27"/>
       <c r="M187" s="27"/>
     </row>
-    <row r="188" spans="2:13" ht="156.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:13" ht="156.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B188" s="7">
         <v>184</v>
       </c>
       <c r="C188" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="D188" s="87"/>
+      <c r="D188" s="66"/>
       <c r="E188" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I188" s="27"/>
       <c r="J188" s="27"/>
-      <c r="K188" s="84"/>
+      <c r="K188" s="63"/>
       <c r="L188" s="27"/>
       <c r="M188" s="27"/>
     </row>
-    <row r="189" spans="2:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:13" ht="114.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B189" s="4">
         <v>185</v>
       </c>
       <c r="C189" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="D189" s="87"/>
+      <c r="D189" s="66"/>
       <c r="E189" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I189" s="27"/>
       <c r="J189" s="27"/>
-      <c r="K189" s="84"/>
+      <c r="K189" s="63"/>
       <c r="L189" s="27"/>
       <c r="M189" s="27"/>
     </row>
-    <row r="190" spans="2:13" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:13" ht="85.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B190" s="7">
         <v>186</v>
       </c>
       <c r="C190" s="53" t="s">
         <v>183</v>
       </c>
-      <c r="D190" s="87"/>
+      <c r="D190" s="66"/>
       <c r="E190" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I190" s="27"/>
       <c r="J190" s="27"/>
-      <c r="K190" s="84"/>
+      <c r="K190" s="63"/>
       <c r="L190" s="27"/>
       <c r="M190" s="27"/>
     </row>
-    <row r="191" spans="2:13" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:13" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B191" s="4">
         <v>187</v>
       </c>
       <c r="C191" s="53" t="s">
         <v>198</v>
       </c>
-      <c r="D191" s="87"/>
+      <c r="D191" s="66"/>
       <c r="E191" s="1" t="s">
         <v>23</v>
       </c>
@@ -4646,127 +4652,127 @@
       </c>
       <c r="I191" s="27"/>
       <c r="J191" s="27"/>
-      <c r="K191" s="84"/>
+      <c r="K191" s="63"/>
       <c r="L191" s="27"/>
       <c r="M191" s="27"/>
     </row>
-    <row r="192" spans="2:13" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:13" ht="99.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B192" s="7">
         <v>188</v>
       </c>
       <c r="C192" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="D192" s="87"/>
+        <v>220</v>
+      </c>
+      <c r="D192" s="66"/>
       <c r="E192" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I192" s="27"/>
       <c r="J192" s="27"/>
-      <c r="K192" s="84"/>
+      <c r="K192" s="63"/>
       <c r="L192" s="27"/>
       <c r="M192" s="27"/>
     </row>
-    <row r="193" spans="2:13" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:13" ht="72" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B193" s="4">
         <v>189</v>
       </c>
       <c r="C193" s="53" t="s">
         <v>199</v>
       </c>
-      <c r="D193" s="87"/>
+      <c r="D193" s="66"/>
       <c r="E193" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I193" s="27"/>
       <c r="J193" s="27"/>
-      <c r="K193" s="84"/>
+      <c r="K193" s="63"/>
       <c r="L193" s="27"/>
       <c r="M193" s="27"/>
     </row>
-    <row r="194" spans="2:13" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:13" ht="71.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B194" s="7">
         <v>190</v>
       </c>
       <c r="C194" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="D194" s="87"/>
+      <c r="D194" s="66"/>
       <c r="E194" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>25</v>
+        <v>221</v>
       </c>
       <c r="I194" s="27"/>
       <c r="J194" s="27"/>
-      <c r="K194" s="84"/>
+      <c r="K194" s="63"/>
       <c r="L194" s="27"/>
       <c r="M194" s="27"/>
     </row>
-    <row r="195" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B195" s="4">
         <v>191</v>
       </c>
       <c r="C195" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="D195" s="87"/>
+      <c r="D195" s="66"/>
       <c r="E195" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I195" s="27"/>
       <c r="J195" s="27"/>
-      <c r="K195" s="84"/>
+      <c r="K195" s="63"/>
       <c r="L195" s="27"/>
       <c r="M195" s="27"/>
     </row>
-    <row r="196" spans="2:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:13" ht="29.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B196" s="7">
         <v>192</v>
       </c>
       <c r="C196" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="D196" s="87"/>
+        <v>210</v>
+      </c>
+      <c r="D196" s="66"/>
       <c r="E196" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I196" s="27"/>
       <c r="J196" s="27"/>
-      <c r="K196" s="84"/>
+      <c r="K196" s="63"/>
       <c r="L196" s="27"/>
       <c r="M196" s="27"/>
     </row>
-    <row r="197" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B197" s="4">
         <v>193</v>
       </c>
       <c r="C197" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="D197" s="87"/>
+      <c r="D197" s="66"/>
       <c r="E197" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I197" s="27"/>
       <c r="J197" s="27"/>
-      <c r="K197" s="84"/>
+      <c r="K197" s="63"/>
       <c r="L197" s="27"/>
       <c r="M197" s="27"/>
     </row>
@@ -4775,10 +4781,10 @@
         <v>194</v>
       </c>
       <c r="C198" s="56" t="s">
-        <v>212</v>
-      </c>
-      <c r="D198" s="82" t="s">
-        <v>214</v>
+        <v>211</v>
+      </c>
+      <c r="D198" s="61" t="s">
+        <v>213</v>
       </c>
       <c r="E198" s="54" t="s">
         <v>23</v>
@@ -4788,7 +4794,7 @@
       </c>
       <c r="I198" s="27"/>
       <c r="J198" s="27"/>
-      <c r="K198" s="84"/>
+      <c r="K198" s="63"/>
       <c r="L198" s="27"/>
       <c r="M198" s="27"/>
     </row>
@@ -4797,9 +4803,9 @@
         <v>195</v>
       </c>
       <c r="C199" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D199" s="83"/>
+        <v>212</v>
+      </c>
+      <c r="D199" s="62"/>
       <c r="E199" s="9" t="s">
         <v>23</v>
       </c>
@@ -4808,7 +4814,7 @@
       </c>
       <c r="I199" s="27"/>
       <c r="J199" s="27"/>
-      <c r="K199" s="84"/>
+      <c r="K199" s="63"/>
       <c r="L199" s="27"/>
       <c r="M199" s="27"/>
     </row>
@@ -4817,9 +4823,9 @@
         <v>196</v>
       </c>
       <c r="C200" s="57" t="s">
-        <v>216</v>
-      </c>
-      <c r="D200" s="83"/>
+        <v>215</v>
+      </c>
+      <c r="D200" s="62"/>
       <c r="E200" s="9" t="s">
         <v>23</v>
       </c>
@@ -4828,7 +4834,7 @@
       </c>
       <c r="I200" s="27"/>
       <c r="J200" s="27"/>
-      <c r="K200" s="84"/>
+      <c r="K200" s="63"/>
       <c r="L200" s="27"/>
       <c r="M200" s="27"/>
     </row>
@@ -4837,9 +4843,9 @@
         <v>197</v>
       </c>
       <c r="C201" s="57" t="s">
-        <v>217</v>
-      </c>
-      <c r="D201" s="83"/>
+        <v>216</v>
+      </c>
+      <c r="D201" s="62"/>
       <c r="E201" s="9" t="s">
         <v>23</v>
       </c>
@@ -4848,7 +4854,7 @@
       </c>
       <c r="I201" s="27"/>
       <c r="J201" s="27"/>
-      <c r="K201" s="84"/>
+      <c r="K201" s="63"/>
       <c r="L201" s="27"/>
       <c r="M201" s="27"/>
     </row>
@@ -4857,9 +4863,9 @@
         <v>198</v>
       </c>
       <c r="C202" s="58" t="s">
-        <v>218</v>
-      </c>
-      <c r="D202" s="83"/>
+        <v>217</v>
+      </c>
+      <c r="D202" s="62"/>
       <c r="E202" s="9" t="s">
         <v>23</v>
       </c>
@@ -4868,7 +4874,7 @@
       </c>
       <c r="I202" s="27"/>
       <c r="J202" s="27"/>
-      <c r="K202" s="84"/>
+      <c r="K202" s="63"/>
       <c r="L202" s="27"/>
       <c r="M202" s="27"/>
     </row>
@@ -4881,6 +4887,14 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="24">
+    <mergeCell ref="D83:D100"/>
+    <mergeCell ref="D101:D123"/>
+    <mergeCell ref="D124:D134"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="D17:D36"/>
     <mergeCell ref="D198:D202"/>
     <mergeCell ref="K186:K197"/>
     <mergeCell ref="K198:K202"/>
@@ -4897,14 +4911,6 @@
     <mergeCell ref="D159:D162"/>
     <mergeCell ref="D37:D49"/>
     <mergeCell ref="D50:D82"/>
-    <mergeCell ref="D83:D100"/>
-    <mergeCell ref="D101:D123"/>
-    <mergeCell ref="D124:D134"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="D17:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>